<commit_message>
Added word seaarch that will return the result with the chapters
</commit_message>
<xml_diff>
--- a/chapters.xlsx
+++ b/chapters.xlsx
@@ -14,399 +14,411 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
   <si>
     <t>Chapter and text</t>
   </si>
   <si>
-    <t>Foreword</t>
-  </si>
-  <si>
     <t>1 Scope</t>
   </si>
   <si>
     <t>2 Normative references</t>
   </si>
   <si>
-    <t>018 1 NORSOK Standard NORSOK S-001:2018 Technical Safety  This NORSOK standard describes the principles and requirements for the development of the physical safety design, i.e. technical safety, of offshore installations for production of oil and gas. Where applicable, this NORSOK standard may also be used for mobile offshore drilling units. This NORSOK standard, together with ISO 1</t>
-  </si>
-  <si>
-    <t>3 Terms and definitions</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> For the purposes of this NORSOK standard, the following terms, definitions and abbreviations apply. .1 shall (requirement) expression in the content of a document conveying objectively verifiable criteria to be fulfilled and from which no deviation is permitted if compliance with the document is to be claimed Note 1 to entry: Requirements are expressed using the verbal forms specified in ISO/IEC Directives, Part  clause 7. Table . . should (recommendation) expression in the content of a document conveying a suggested possible choice or course of action deemed to be particularly suitable without necessarily mentioning or excluding others NORSOK S-001:018 4 NORSOK © 018 Note 1 to entry: Recommendations are expressed using the verbal forms specified in ISO/IEC Directives, Part  clause 7. Table 4. Note  to entry: In the negative form, a recommendation is the expression that a suggested possible choice or course of action is not preferred but it is not prohibited. . may (permission) expression in the content of a document conveying consent or liberty (or opportunity) to do something Note 1 to entry: Permissions are expressed using the verbal forms specified in ISO/IEC Directives Part  clause 7.4 Table 5. .4 can (possibility and capability) 1: expression in the content of a document conveying expected or conceivable material, physical or causal outcome. : expression in the content of a document conveying the ability, fitness, or quality necessary to do or achieve a specified thing Note 1 to entry: Possibility and capability is expressed using the verbal forms specified in in ISO/IEC Directives, Part  clause 7.5 Table 6. .5 area classification division of an installation into hazardous areas and non-hazardous areas and the sub-division of hazardous zones under normal operation. Note 1 to entry: Normal operation is a situation when the plant is operating within its design parameters. Minor releases of flammable material may be part of normal operation. For example, releases from seals that rely on wetting by the fluid being pumped are considered to be minor releases. Failures (such as breakdown of pump seals, flange gaskets or spillage caused by accidents) that involve repair or shutdown are not considered to be part of normal operation, and may require special precautions of potential ignition sources. .6 design accidental load accidental load/action used as a basis for design Note 1 to entry: The design load/action can be the same as the dimensioning accidental load/action, but it can be higher, based on different input and assessments such as ALARP, minimum requirements in the regulations etc. .7 design fire the design fire for load bearing structures and fire divisions includes as a minimum: the dimensioning fire worst credible process fire fire class requirements, e.g. H-class .8 detection area area, or areas, of similar environmental and operating conditions and hazards, and with similar detection and protection arrangements. NORSOK S-001:018 NORSOK © 018 5 Note 1 to entry: For HC areas, the detection area is normally similar to the fire area in question. Very large fire areas may exceptionally be split into two or more detection areas, e.g. large tank decks on FPSOs. Each detection area will have a C&amp;E Diagram, e.g. FPDS. .9 dimensioning accidental load an accidental load/action that a function or a system shall be able to withstand for a given period of time to meet the defined acceptance criteria for risk .10 dimensioning gas cloud the minimum stoichiometric gas cloud which, when ignited, can create an explosion resulting in an explosion pressure exceeding the dimensioning explosion load of the area .11 escape route route from an area of an installation leading to a muster or embarkation area. .1 essential equipment equipment that shall be kept alive to maintain production or drilling/well operations. Note 1 to entry: Such equipment may include main power generator, main electrical distribution panels, diesel engines, heaters, boilers ventilation systems, unless defined as a safety critical item .1 evacuation planned method of leaving the installation in an emergency situation .14 evaluation a simplified assessment which does not require to be documented in a separate analysis or study report Note 1 to entry: The reasoning and conclusions should be described e.g. in the safety strategy. .15 explosion load the load generated by combustion of a flammable gas or mist which generates pressure and drag effects .16 fire area area separated from other areas either by physical barriers (fire/blast division) or sufficient distance which will prevent a fire or explosion to spread to another fire area when exposed to the design loads. .17 fire load time and space dependent radiative and convective heat load from a fire .18 fire water (FW) pump system total system which supplies water for firefighting system Note 1 to entry: i.e. water inlets with filters, FW pumps, risers, power sources, power transmissions, fuel pipes/tanks and control systems NORSOK S-001:018 6 NORSOK © 018 .19 hazardous area an area in which a flammable atmosphere is or may be expected to be present in quantities such as to require special precautions for the control of potential ignition sources .0 ignition Source equipment and activities which may under certain circumstances cause ignition of an explosive atmosphere Note 1 to entry: Typically ignition sources relate to the following type of equipment; non Ex-certified electrical equipment (or not approved for Zone ), open flames, direct heat and hot surfaces, rotating machinery and combustion engines, mechanical sparks, static electricity, radio frequency energy, chemical reaction (e.g. iron sulphide). Note  to entry: Electrical equipment will not constitute an ignition source if in compliance with relevant IEC zone requirements or better. .1 ignition source groups Group 1 (non-essential equipment): non-explosion protected equipment which is not affecting production availability or safety integrity. Group  (essential equipment): non-explosion protected equipment which shall be kept alive to maintain production and drilling operation. Group  (safety critical equipment): non-explosion protected equipment that shall be in operation to ensure rescue and medical treatment of injured personnel, escape and evacuation, prevent escalation or bring the installation to a safe state. . inhibit disabling of the safety instrumented function input and prevention of a shutdown action; Note 1 to entry: e.g. by disabling of the input signal to the shutdown logic while still presenting the alarm to the operator . intermittently manned work area or work place where inspection, maintenance or other work is planned to last at least  h, but less than 8 h a day for at least 50 % of the installation™s operation time .4 local equipment room (LER a room containing electrical and instrumentation equipment .5 main area area that includes similar functions on the installation. Note 1 to entry: Main areas can be the: a) living quarter b) utility area c) drilling area d) wellhead area e) process area f) storage area for hydrocarbons Note  to entry: Drilling and wellhead area may be combined. See subclause 0.4.1. NORSOK S-001:018 NORSOK © 018 7 .6 muster area designated area where mustering shall take place in the event of general and/or evacuation alarm, and where personnel is sheltered while emergency response and evacuation pre-planning are undertaken .7 non-essential equipment any equipment not affecting production availability or safety integrity .8 non-hazardous area all areas not classified as hazardous under normal operation .9 normally not manned area work area or work place that is not permanently or intermittently manned. .0 normally not manned installations installations that can be left unmanned and still maintain their intended function through remote control .1 override disabling of the safety instrumented function output and prevention of a shutdown action, e.g. by disabling the signal from shutdown logic to an individual shutdown output action. . permanently manned work area or work place manned at least 8 hours a day for at least 50 % of the installations operation time . safety critical equipment equipment that shall be in operation to ensure rescue and medical treatment of injured personnel, escape and evacuation, prevent escalation or bring the installation to a safe state, Note 1 to entry: e.g. equipment powered from UPS and/or emergency generator(s), fire water pump drivers, etc. Ignition source Group , see definition, is a sub-group of this equipment. .4 well barrier envelope of one or several barrier elements preventing well fluids from flowing unintentionally from the formation into another formation or to surface. 4 </t>
-  </si>
-  <si>
-    <t>4 Abbreviations</t>
-  </si>
-  <si>
-    <t>:01, Helicopter Deck on Offshore Installations NORSOK D-001, Drilling facilities NORSOK D-010, Well integrity in drilling and well operations NORSOK H-00, Heating, ventilation and air conditioning (HVAC) and sanitary systems NORSOK L-001, Piping and valves NORSOK L-00, Piping design, layout and stress analysis NORSOK L-00</t>
-  </si>
-  <si>
-    <t>5 Management of technical safety</t>
+    <t>017 NORSOK © 2017 1 NORSOK Standard N-00</t>
+  </si>
+  <si>
+    <t>3 Terms, definitions and abbreviations</t>
   </si>
   <si>
     <t xml:space="preserve"> .1 </t>
   </si>
   <si>
+    <t>3.1 Terms and definitions</t>
+  </si>
+  <si>
+    <t>3.2 Abbreviations</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ............................................................................................................................... 9 4 </t>
+  </si>
+  <si>
+    <t>4 Permanent actions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ..................................................................................................................................................... 6  ............................................................................................................................. 6  Termer, definitions and abbreviations .................................................................................................... 6 .1  ................................................................................................................... 6 .  ............................................................................................................................... 9 4  ............................................................................................................................... 10 </t>
+  </si>
+  <si>
+    <t>4.1 General</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ...................................................................................................................................... 10 . </t>
+  </si>
+  <si>
+    <t>4.2 Hydrostatic pressure difference</t>
+  </si>
+  <si>
+    <t>5 Variable functional actions</t>
+  </si>
+  <si>
     <t>5.1 General</t>
   </si>
   <si>
-    <t>5.2 Activities related to technical safety design</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>5.2.1 Overview</t>
-  </si>
-  <si>
-    <t>5.2.2 Define context</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Context needs to be defined and compiled so that frame conditions, limitations and ambitions for the installation (and its areas and activities) are available for relevant personnel involved in technical safety issues or technical safety management. Examples of context are legislation, standards (internal/ external), concept decisions, operating conditions, prerequisites for use, assumptions/ requirements and NORSOK S-001:018 NORSOK © 018 11 demands to risk reduction. The context applied for the management of technical safety has to be traceable and documented. A major part of the context will be defined early in the development of an installation. During the installation life cycle the context will provide a basis for use/ reassessment and it need to be updated to ensure that all relevant changes and modifications are included. </t>
-  </si>
-  <si>
-    <t>5.2.3 Identify hazards and accidental events (HAZID)</t>
-  </si>
-  <si>
-    <t>5.2.4 Perform risk analyses and evaluations</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Risk and safety analyses / studies shall be performed to establish sufficiently detailed information about the risk associated with the identified hazards and accidental events. The information will be used to evaluate the risk and to decide which solutions (barriers), and related requirements that are needed for preventing, controlling and mitigating the hazards in addition to generic requirements given by the context. Evaluation of risk includes an assessment of: compliance with predefined evaluation criteria (e.g. minimum requirements and acceptance criteria in context); necessary ALARP processes to demonstrate that risk has been reduced to a level as low as reasonably practicable; uncertainties associated with the hazards, accidental events and their consequences as well as the risk reducing effect of the barriers. The results from risk analyses are used for many purposes. One is to provide information and decision support related to the need for and role of risk reducing measures (barriers) and their required performance. Another is to provide decision support regarding the risk level assessed and if this is considered acceptable for the facility. Reference is made to subclause .10 for examples of studies and evaluations. For a development project, the degree of details in the risk and safety analyses / studies will increase as the project matures through different phases. Thus, solutions, assumptions and conservative estimates typically used in early stages may be verified or changed due to more detailed analyses. </t>
-  </si>
-  <si>
-    <t>5.2.5 Identify and define barrier functions, systems and elements (risk treatment)</t>
-  </si>
-  <si>
-    <t>5.2.6 Safety strategies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Documentation shall be prepared to record how specific hazards or accidental events are managed by the use of barrier functions, systems and elements. This documentation can be denoted the 'safety strategy™ (or ‚the barrier strategy™) and can replace the need for Fire and Explosion Strategy (FES) and the Escape, Evacuation and Rescue Strategy (EER strategy) as required by ISO 170. Safety strategies do not necessarily need to be described in a single document. The strategy may be described and included in other relevant documentation where this is natural and appropriate. The need to develop separate strategies can be viewed in relation to the other documentation which exists or is prepared for the individual facility. Safety strategy documentation should also be prepared to outline applicable overall principles for design, layout, arrangement, philosophies and other high-level design and operational aspects related to barriers; e.g.: how different safety documentation are linked together; risk reduction principles - inherent safety design; premises for design; design provisions for the operating phase; accidental loads and resistance. </t>
-  </si>
-  <si>
-    <t>5.2.7 Define performance requirements</t>
-  </si>
-  <si>
-    <t>5.2.8 Define performance Standards</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> It may be beneficial to group the various performance requirements into performance standards including a description of the role of the safety functions. Dependencies on and interfaces with other systems should also be described. </t>
-  </si>
-  <si>
-    <t>5.2.9 Establish safety requirement specification (SRS)</t>
-  </si>
-  <si>
-    <t>5.2.10 Safety specifications, diagrams, drawings, philosophies, etc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">. Documentation that needs to be developed to deepen or clarify performance requirements when necessary. Ref. subclause .10 Documentation. Also, see Annex C for proposed format and information for data sheets for selected Safety Equipment. . </t>
-  </si>
-  <si>
-    <t>5.3 Risk reduction principles and inherent safety design</t>
-  </si>
-  <si>
-    <t>5.4 Design provisions for the operating phase</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Effective management of technical barriers in project development and design processes also need to address relevant dependencies with operational and organizational aspects for the operating phase. Some examples of interfaces between technical, operational and organizational aspects to be considered are: operational prerequisites for start-up and use; measures and restrictions that are necessary in the event of overriding, disconnection or in the event of missing/impaired safety systems and barriers; maintenance; competence; emergency preparedness; manual intervention. In order to ensure solutions which are suited for varying conditions, particular prerequisites shall be accommodated for in the design phase (and sustained during the operating phase). Examples of aspects that should be addressed are: assumptions including conditions and possible actions, when operating in different modes, i.e. normal, test, fault, failure, degraded. (Relevant assumptions in risk analyses should be according to requirements in the different installation specific performance standards); NORSOK S-001:018 NORSOK © 018 1 provisions, routines and logs for isolation of safety related functions during testing and maintenance, e.g. by inhibit (disabling input signal) and override (disabling output action). Such isolation should not render unnecessarily large parts of the system inactive. Logging, manual or automatic, of any such isolation action, e.g. time, number and duration, is mandatory; requirements for compensatory measures. (Responsible personnel for the operating phase will need to implement the necessary measures to remedy or compensate for non-conformities, missing or impaired barriers). The basis for inspection, testing and maintenance shall be described as part of project development in close liaison with the end user and be finalized before start-up. Important elements are: Systems, equipment and barriers shall be classified as regards the health, safety and environment consequences of potential functional failures. Information in performance standards shall regardless of other criticality analyses (e.g. according to NORSOK Z-008) be used as basis for categorizing safety critical equipment. An inspection-, testing- and maintenance programme for safety barriers shall be developed as part of project development. The programme should include test/inspection/maintenance methods and intervals. These shall be determined based upon regulatory requirements, company requirements, performance requirements, results/assumptions from analyses (e.g. SIL), criticality analysis (ref NORSOK Z-008), manufacturers™ recommendations, operating experience and relevant plant maintenance strategy. For instrumented safety systems, also see Norwegian Oil and Gas Association GL070. For structures, see NORSOK N-00. The safety functions/systems should, where reasonably practicable, allow for the required testing to be carried out without interrupting production or operations. Systems shall be established for monitoring barrier integrity, including possible deficiencies and degradation. The system should be established and populated with data during commissioning. . </t>
-  </si>
-  <si>
-    <t>5.5 Commissioning and start-up</t>
-  </si>
-  <si>
-    <t>5.6 Accidental loads and resistance</t>
-  </si>
-  <si>
-    <t>5.6.1 General</t>
-  </si>
-  <si>
-    <t>5.6.2 Gas explosions</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Explosion loads from ignited gas clouds are strongly dependent on factors such as: cloud size and gas concentration; gas type; confinement and/or congestion of the affected area; explosion relief solutions; ignition location. Design explosion loads shall be established using a recognised method (e.g. NORSOK Z-01) and a representative geometric explosion model with representative equipment density. It is recognized that in the initial design the detail arrangement may not have been developed. An explosion study should be performed at an early stage, enabling the key installation parts to be located favorably with regard to explosion. The methods and detailing of the input will reflect this situation. Explosion loads shall be defined for relevant horizontal and vertical area dividers (pressure and impulse from explosion) and relevant equipment (pressure/drag forces). Explosion loads shall also be defined for areas external to the initial explosion location (typical LQ, utility modules etc.) if applicable. Equipment that can become a flying object and can significantly impair critical safety equipment/structures such as fire divisions, riser valves, wellheads, blowdown piping, should be considered secured. Examples of such equipment are well hatches, panels, temporary equipment, etc. </t>
-  </si>
-  <si>
-    <t>5.6.3 Hydrocarbon fires</t>
-  </si>
-  <si>
-    <t>5.6.3.1 General</t>
-  </si>
-  <si>
-    <t>5.6.3.2 Main load bearing structures</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> For main load bearing structures, the heat load distribution is of great importance. A validated computational fluid dynamics (CFD) model shall be used to provide realistic modelling of the fire source and the effect of the surroundings in order to define the design accidental load. Care shall be taken when selecting simulation cases. Either these shall be selected and used conservatively, or a larger number of simulations are necessary to be statistically representative. .6.. </t>
-  </si>
-  <si>
-    <t>5.6.3.3 Worst credible process fire</t>
-  </si>
-  <si>
-    <t>5.6.3.4 Unacceptable ruptures of process equipment in a fire situation.</t>
-  </si>
-  <si>
-    <t>5.6.3.5 Process equipment and piping – fire calculations</t>
-  </si>
-  <si>
-    <t>5.7 Qualification of technology</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Technology that requires qualification is defined as systems or components for which an acceptable reliability is not demonstrated by a documented track record for the particular application. The technology shall be qualified following a systematic approach, such as laid down in DNV-RP-A0 [1] or similar guideline, in order to demonstrate that it meets specified functional requirements and reliability targets. .8 </t>
-  </si>
-  <si>
-    <t>5.8 Experience transfer</t>
-  </si>
-  <si>
-    <t>5.9 Temporary equipment</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Temporary equipment shall be in accordance with NORSOK Z-01 Temporary Equipment and follow the relevant principles of this document, e.g. survivability of safety critical equipment and ignition source control. For temporary equipment operated as self-contained units, well completion and workover units etc, the interfaces shall be considered in the design phase both for normal and emergency situations, e.g., available power to secure operations in emergency situations and ignition source control. Main lay-down areas should be prepared for connection of containers and temporary equipment to the platform™s Fire &amp; Gas system. .10 </t>
-  </si>
-  <si>
-    <t>5.10 Documentation</t>
-  </si>
-  <si>
-    <t>6 Layout</t>
-  </si>
-  <si>
-    <t>6.1 Role</t>
-  </si>
-  <si>
-    <t>6.2 Interfaces</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  and arrangement including explosion barriers will interact with design and performance of other safety systems and barriers. . </t>
-  </si>
-  <si>
-    <t>6.3 Required utilities</t>
-  </si>
-  <si>
-    <t>6.4 Functional requirements</t>
-  </si>
-  <si>
-    <t>6.4.1 Main design principles</t>
-  </si>
-  <si>
-    <t>6.4.2 Riser flow line area</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hydrocarbon risers and associated equipment shall be designed and located to minimise risk due to accidental events (such as gas leakages, fires, explosions, ship impact and dropped objects), including accidents where riser or associated equipment is the initial source. Pig launchers and receivers shall be located in open naturally ventilated areas at the periphery of the platform facing sea, and with hatches directed away from equipment and structures. It shall not be possible to open pressurized pig launchers/receivers. NORSOK S-001:018  NORSOK © 018 Risers and riser ESD valves shall be located or protected to minimize the likelihood of damage below the ESD valves causing release of pipeline/riser inventories. The riser shall be protected against design accidental loads. Reference is also made to subclause 8.. for other riser requirements. The riser ESD valves shall be located as close to sea-level as practicable, i.e. cellar deck or lower. Riser ESD valves should be located in open, naturally ventilated area and such that liquid accumulation below the valve is avoided. </t>
-  </si>
-  <si>
-    <t>6.4.3 Process area</t>
-  </si>
-  <si>
-    <t>6.4.4 Well areas</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Drilling risers and conductors shall be designed and positioned or protected to minimize the likelihood of damage, including that due to ship impact and dropped objects. For installations with main support frame (MSF), the wellheads should be located above the MSF in order to reduce exposure of the MSF from a wellhead fire. </t>
-  </si>
-  <si>
-    <t>6.4.5 Piping</t>
-  </si>
-  <si>
-    <t>6.4.6 Lifting and lay down</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Crane coverage and lay down areas shall be arranged to promote safe crane operations with free visibility from crane cabin and minimise the risk of dropped objects. Considerations shall be given to sidewise movement of load. Within defined lifting zones equipment, or piping, containing hydrocarbons, flammable or toxic gas/liquid shall be protected from dropped objects. Lifting above high voltage equipment and cables shall be assessed, and protection shall be considered installed. The lifting zones shall be defined and shown on the lifting map in crane cabin. Crane software should give alarm in crane when lifting restriction boundaries are exceeded. Allowable weight chart for laydown areas shall be established. Laydown and storage area should not be located in hazardous area. Location of laydown areas and temporary storage of equipment shall be considered to minimize effect on explosion overpressure, ventilation, flying debris from explosions and possible negative effects on technical barriers (e.g. F&amp;G detection, FW system, natural ventilation). Reference is made to NORSOK R-00 for further details. </t>
-  </si>
-  <si>
-    <t>6.4.7 Storage and handling of explosives</t>
-  </si>
-  <si>
-    <t>6.4.8 Floating installations</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> For floating installations, the following shall apply: Systems with hydrocarbons with flashpoint below 0 °C shall not be installed in columns or pontoons for floating installations. Storage of diesel in atmospheric tanks is acceptable. NORSOK S-001:018  NORSOK © 018 Vital control functions (e.g. maritime control/bridge, process control and special emergency preparedness functions) shall be arranged in one common control centre for the entire installation.  shall be separated from FPSO hydrocarbon storage tank top by air gap of minimum  m and plated deck and bunding in order to avoid hydrocarbons spreading to the storage tank deck. Reference is made to 1.. with respect to fire protection of tank deck. Equipment that can represent an ignition source (e.g. exhaust ducts and generators) should be located upwind of potential leak sources on floating installation that will be turned up against the wind. The effects of 'green sea' shall be carefully evaluated and means of protection arranged. Submerged crude pumps shall be used for FPSOs. If submerged pumps are not selected for FSUs, the decision shall be supported by a safety study. Crude oil transfer lines or any other hydrocarbon line shall not be located in double bottom. </t>
-  </si>
-  <si>
-    <t>6.4.9 Turret</t>
-  </si>
-  <si>
-    <t>6.4.10 Explosion design principles</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The amount of explosion relief available, the degree of blockage and congestion in an area of an explosion shall be optimised to reduce explosion risk. Design principles in ISO 170, A., B.1, B.10 to B.11, should be followed. The use of explosion panels and weather protection shields shall be kept to a minimum. Natural ventilation and open modules shall be preferred. Where such arrangements are likely to cause an unacceptable working environment, special solutions such as temporary shields for maintenance operations should be considered. The arrangement of equipment in an area, and particularly near ventilation openings, can have a major influence on the peak overpressures expected in an area. Cable trays, junction boxes, piping and equipment shall be located so that they will not significantly increase turbulence, block explosion ventilation openings and reduce the free vent area, and thus increase explosion loads. </t>
-  </si>
-  <si>
-    <t>6.4.11 Hot air exposure of helicopter deck</t>
-  </si>
-  <si>
-    <t>6.5 Survivability requirements</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Equipment with a safety function, during and after the accident, shall generally be located and protected such that its role and function are maintained. 7 </t>
-  </si>
-  <si>
-    <t>7 Structural integrity</t>
-  </si>
-  <si>
-    <t>0, defines the required standard to establish and maintain an adequate level of safety for personnel, environment and material assets.  The following standards include provisions and guidelines which, through reference in this text, constitute provisions and guidelines of this NORSOK standard. Latest issue of the references shall be used unless otherwise agreed. Other recognized standards may be used provided it can be shown that they meet the requirements of the referenced standards. NORSOK C-001, Living quarters area NORSOK C-00:01, Architectural components and equipment NORSOK C-00:01, Helicopter Deck on Offshore Installations NORSOK D-001, Drilling facilities NORSOK D-010, Well integrity in drilling and well operations NORSOK H-00, Heating, ventilation and air conditioning (HVAC) and sanitary systems NORSOK L-001,  and valves NORSOK L-00,  design, layout and stress analysis NORSOK L-00, Compact flanged connections NORSOK N-001, Structural design NORSOK N-00, Actions and action effects NORSOK N-00, In-service integrity management of structures and maritime systems NORSOK P-00, Process System Design NORSOK R-00, Lifting Equipment NORSOK T-001, Telecom Systems NORSOK T-100, Telecom Subsystems NORSOK Z-008, Risk based maintenance and consequence classification NORSOK Z-01, Risk and emergency preparedness analysis NORSOK Z-01, Temporary Equipment NORSOK S-001:018  NORSOK © 018 CENELEC CLC/TR 07, Assessment of inadvertent ignition of flammable atmospheres by radio-frequency radiation EN  all parts, Fire Detection and Alarm Systems EN 0, Respiratory protective devices for self-rescue - Filtering devices with hood for escape from fire - Requirements, testing, marking EN 117-1, Explosive atmospheres - Explosion prevention and protection - Part 1: Basic concepts and methodology EN 188, Lighting applications Œ Emergency lighting EN 1-1, Industrial valves - Testing of metallic valves - Part 1: Pressure tests, test procedures and acceptance criteria - Mandatory requirements EN 1-, Industrial valves - Testing of metallic valves - Part : Tests, test procedures and acceptance criteria - Supplementary requirements EN 8 Management of alarms systems for the process industries ISO 1018:00/AC:009, Petroleum and natural gas industries Œ Offshore production installations Œ Basic surface process safety systems ISO 10, Petroleum and natural gas industries - Drilling and production equipment - Wellhead and christmas tree equipment ISO 1097, Testing of valves - Fire type-testing requirements ISO 170:01, Petroleum and natural gas industries Œ Control and mitigation of fires and explosions on offshore production installations Œ Requirements and guidelines ISO 118, Petroleum and natural gas industries - Offshore production installations - Heating, ventilation and air-conditioning ISO 109, Graphical Symbols Œ Safety Signs -- Safety Way Guidance System (SWGS) ISO 899, Determination of the resistance to jet fires of passive fire protection materials -- Part 1:  requirements ISO 80079-. Explosive atmospheres - Part : Non-electrical equipment for explosive atmospheres - Basic method and requirements IEC 0079(part 10, part 1:01/COR1:01 and part 9), Explosive atmospheres IEC 01(all parts), Tests for electric cables under fire conditions Œ Circuit integrity IEC 108(all parts), Functional safety of electrical/electronic/programmable electronic safety-related systems IEC 111(all parts), Functional safety Œ Safety instrumented systems for the process industry sector IEC 189(parts 1, , , , :01 and 7) Mobile and fixed offshore units Œ Electrical installations API RP 1C:017, Recommended Practice for Analysis, Design, Installation, and Testing of Basic Surface Safety Systems for Offshore Production Platforms (8th ed) API Spec 17J, Specification for Unbonded Flexible Pipe API STD 0, Sizing, Selection, and Installation of Pressure-relieving Devices API STD 1, Pressure-Relieving and Depressurizing Systems Directive 9/9/EC, Concerning equipment and protective systems intended for use in potentially explosive atmospheres (ATEX ﬁProductﬂ) DNVGL-ST-E0, Design of Free Fall Lifeboats DNVGL-ST-F01, Dynamic risers NORSOK S-001:018 NORSOK © 018  EEMUA 191 Alarm systems - a guide to design, management and procurement EI 1, Model code of safe practice Part 1: Area classification code for installations handling flammable fluids LSA Code, IMO SOLAS Life saving appliances (LSA) Code, adopted by the Maritime Safety Committee by resolution MSC.8 () Norwegian Oil and Gas Association GL0, Anbefalte retningslinjer for etablering av områdeberedskap Norwegian Oil and Gas Association GL070, Guidelines for the Application of IEC 108 and IEC 111 in the petroleum activities on the continental shelf Norwegian Oil and Gas Association GL07, Anbefalte retningslinjer for vannbaserte brannbekjempelsessystemer Norwegian Oil and Gas Association GL09, Kravspesifikasjoner for redningsdrakt til bruk på norsk kontinentalsokkel. MODU Code, Code for the construction and equipment of mobile offshore drilling units NFPA 11, Standard for Low-, Medium-, and High-Expansion Foam NFPA 1, Installation of Sprinkler Systems NFPA 1, Standard for the Installation of Standpipe and Hose Systems NFPA 1, Standard for Water Spray Fixed Systems for Fire Protection NFPA 1, Standard for the Installation of Foam-Water Sprinkler and Foam-Water Spray Systems NFPA 0, Standard for the Installation of Stationary Fire Pumps for Fire Protection Spray Systems NFPA 70, Standard on Water Mist Fire Protection Systems NMA Regulations No.7, Regulation concerning ballast systems on mobile offshore units (Ballast Regulations) NMA Regulations No. 90, Evacuation and Life-saving appliances on mobile offshore units NMA Regulations No. 1, Regulation for mobile offshore units with production plants and equipment NMA Regulations No. 998, Regulation concerning positioning and anchoring systems on mobile offshore units   For the purposes of this NORSOK standard, the following terms, definitions and abbreviations apply. .1 shall (requirement) expression in the content of a document conveying objectively verifiable criteria to be fulfilled and from which no deviation is permitted if compliance with the document is to be claimed Note 1 to entry: Requirements are expressed using the verbal forms specified in ISO/IEC Directives, Part  clause 7. Table . . should (recommendation) expression in the content of a document conveying a suggested possible choice or course of action deemed to be particularly suitable without necessarily mentioning or excluding others NORSOK S-001:018  NORSOK © 018 Note 1 to entry: Recommendations are expressed using the verbal forms specified in ISO/IEC Directives, Part  clause 7. Table . Note  to entry: In the negative form, a recommendation is the expression that a suggested possible choice or course of action is not preferred but it is not prohibited. . may (permission) expression in the content of a document conveying consent or liberty (or opportunity) to do something Note 1 to entry: Permissions are expressed using the verbal forms specified in ISO/IEC Directives Part  clause 7. Table . . can (possibility and capability) 1: expression in the content of a document conveying expected or conceivable material, physical or causal outcome. : expression in the content of a document conveying the ability, fitness, or quality necessary to do or achieve a specified thing Note 1 to entry: Possibility and capability is expressed using the verbal forms specified in in ISO/IEC Directives, Part  clause 7. Table . . area classification division of an installation into hazardous areas and non-hazardous areas and the sub-division of hazardous zones under normal operation. Note 1 to entry: Normal operation is a situation when the plant is operating within its design parameters. Minor releases of flammable material may be part of normal operation. For example, releases from seals that rely on wetting by the fluid being pumped are considered to be minor releases. Failures (such as breakdown of pump seals, flange gaskets or spillage caused by accidents) that involve repair or shutdown are not considered to be part of normal operation, and may require special precautions of potential ignition sources. . design accidental load accidental load/action used as a basis for design Note 1 to entry: The design load/action can be the same as the dimensioning accidental load/action, but it can be higher, based on different input and assessments such as ALARP, minimum requirements in the regulations etc. .7 design fire the design fire for load bearing structures and fire divisions includes as a minimum: the dimensioning fire worst credible process fire fire class requirements, e.g. H-class .8 detection area area, or areas, of similar environmental and operating conditions and hazards, and with similar detection and protection arrangements. NORSOK S-001:018 NORSOK © 018  Note 1 to entry: For HC areas, the detection area is normally similar to the fire area in question. Very large fire areas may exceptionally be split into two or more detection areas, e.g. large tank decks on FPSOs. Each detection area will have a C&amp;E Diagram, e.g. FPDS. .9 dimensioning accidental load an accidental load/action that a function or a system shall be able to withstand for a given period of time to meet the defined acceptance criteria for risk .10 dimensioning gas cloud the minimum stoichiometric gas cloud which, when ignited, can create an explosion resulting in an explosion pressure exceeding the dimensioning explosion load of the area .11 escape route route from an area of an installation leading to a muster or embarkation area. .1 essential equipment equipment that shall be kept alive to maintain production or drilling/well operations. Note 1 to entry: Such equipment may include main power generator, main electrical distribution panels, diesel engines, heaters, boilers ventilation systems, unless defined as a safety critical item .1 evacuation planned method of leaving the installation in an emergency situation .1 evaluation a simplified assessment which does not require to be documented in a separate analysis or study report Note 1 to entry: The reasoning and conclusions should be described e.g. in the safety strategy. .1 explosion load the load generated by combustion of a flammable gas or mist which generates pressure and drag effects .1 fire area area separated from other areas either by physical barriers (fire/blast division) or sufficient distance which will prevent a fire or explosion to spread to another fire area when exposed to the design loads. .17 fire load time and space dependent radiative and convective heat load from a fire .18 fire water (FW) pump system total system which supplies water for firefighting system Note 1 to entry: i.e. water inlets with filters, FW pumps, risers, power sources, power transmissions, fuel pipes/tanks and control systems NORSOK S-001:018  NORSOK © 018 .19 hazardous area an area in which a flammable atmosphere is or may be expected to be present in quantities such as to require special precautions for the control of potential ignition sources .0 ignition Source equipment and activities which may under certain circumstances cause ignition of an explosive atmosphere Note 1 to entry: Typically ignition sources relate to the following type of equipment; non Ex-certified electrical equipment (or not approved for Zone ), open flames, direct heat and hot surfaces, rotating machinery and combustion engines, mechanical sparks, static electricity, radio frequency energy, chemical reaction (e.g. iron sulphide). Note  to entry: Electrical equipment will not constitute an ignition source if in compliance with relevant IEC zone requirements or better. .1 ignition source groups Group 1 (non-essential equipment): non-explosion protected equipment which is not affecting production availability or safety integrity. Group  (essential equipment): non-explosion protected equipment which shall be kept alive to maintain production and drilling operation. Group  (safety critical equipment): non-explosion protected equipment that shall be in operation to ensure rescue and medical treatment of injured personnel, escape and evacuation, prevent escalation or bring the installation to a safe state. . inhibit disabling of the safety instrumented function input and prevention of a shutdown action; Note 1 to entry: e.g. by disabling of the input signal to the shutdown logic while still presenting the alarm to the operator . intermittently manned work area or work place where inspection, maintenance or other work is planned to last at least  h, but less than 8 h a day for at least 0 % of the installation™s operation time . local equipment room (LER a room containing electrical and instrumentation equipment . main area area that includes similar functions on the installation. Note 1 to entry: Main areas can be the: a) living quarter b) utility area c) drilling area d) wellhead area e) process area f) storage area for hydrocarbons Note  to entry: Drilling and wellhead area may be combined. See subclause 0..1. NORSOK S-001:018 NORSOK © 018 7 . muster area designated area where mustering shall take place in the event of general and/or evacuation alarm, and where personnel is sheltered while emergency response and evacuation pre-planning are undertaken .7 non-essential equipment any equipment not affecting production availability or safety integrity .8 non-hazardous area all areas not classified as hazardous under normal operation .9 normally not manned area work area or work place that is not permanently or intermittently manned. .0 normally not manned installations installations that can be left unmanned and still maintain their intended function through remote control .1 override disabling of the safety instrumented function output and prevention of a shutdown action, e.g. by disabling the signal from shutdown logic to an individual shutdown output action. . permanently manned work area or work place manned at least 8 hours a day for at least 0 % of the installations operation time . safety critical equipment equipment that shall be in operation to ensure rescue and medical treatment of injured personnel, escape and evacuation, prevent escalation or bring the installation to a safe state, Note 1 to entry: e.g. equipment powered from UPS and/or emergency generator(s), fire water pump drivers, etc. Ignition source Group , see definition, is a sub-group of this equipment. . well barrier envelope of one or several barrier elements preventing well fluids from flowing unintentionally from the formation into another formation or to surface.   For this document, the following abbreviations apply. AC/h air changes per hour AFP active fire protection AIS automatic identification system API American Petroleum Institute NORSOK S-001:018 8 NORSOK © 018 APS abandon platform shutdown ASV annular safety valve ASME American Society of Mechanical Engineers ATEX Atmosphères Explosibles (forskrift om utstyr og sikkerhetssystem til bruk i eksplosjonsfarlig område) BOP blow out preventer C&amp;E cause and effect CAP critical action panel CCR central control room DHSV down hole safety valve DIFFS deck integrated firefighting system EDP Emergency Depressurisation EER evacuation, escape and rescue EN European Standard ESD emergency shutdown F&amp;G fire and gas FPDS fire protection data sheet FPSO floating production, storage and offloading FSU floating storage unit FW fire water HC hydrocarbon HMI human machine interface HVAC heating, ventilation and air conditioning IEC International Electrotechnical Commission IMO International Maritime Organisation IDLH Immediate Danger to Life and Health ISC ignition source control ISO International Organization for Standardization IR infrared LAHH level alarm high high (trip level) LCS loading computer system LEL lower explosive limit LELm lower explosive limit meters LER local equipment room LIR local instrument room LQ living quarter MCP manual call point MOB man over board NORSOK S-001:018 NORSOK © 018 9 MODU mobile offshore drilling unit MV master valve NA not applicable NFPA National Fire Protection Association NMA Norwegian Maritime Authority NNMI normally not manned installations PA public address PAGA public address and general alarm PFD probability of failure on demand PFP passive fire protection PSD process shutdown PSV pressure safety valve RIO Remote input/output SAS safety and automation system SIL safety integrity level SOLAS International Convention for the Safety of Life at Sea SSIV subsea isolation valve UHF ultra high frequency VDU visual display unit UPS uninterruptible power supply VHF very high frequency WV wing valve   .1  Technical safety management (loss prevention) in project development comprises activities to identify risks and to develop and document safety strategies and performance requirements for safety systems and barriers. These are iterative processes as the project develops and design matures. Necessary supporting documentation (e.g. studies, analysis and design reviews) shall be provided with due consideration for timely input to design and procurement processes. Concepts combining a jack-up drilling rig and a fixed installation require special consideration, ref. aspects described in Annex A - Jack-up/jacket constellations. A follow-up system shall be established that enables proper documentation, handling, follow-up and closeout of agreed actions and recommendations from the various studies and analyses in the project. In the event space is allocated for future expansions in new project developments, the design should incorporate sufficient flexibility to include capacity for the additional equipment, e.g. fire water, flare etc. fire water. NORSOK S-001:018 10 NORSOK © 018 For modification projects (e.g. upgrading of existing installation/module, tie-in of satellite field), technical safety management activities adjusted to project scope and complexity shall be performed, including new analyses or updating of existing analyses for factors that are affected by the modification. The individual project or installation shall perform specific hazard identification and risk analysis and evaluation processes. Based on this process, the requirements in this document shall be supplemented as necessary to manage the risk. .   A flow diagram illustrating some of the main activities related to technical safety design is shown in Figure 1. The activities are detailed in the immediate following subclauses. Reference is made to NORSOK Z-01 for details related to risk assessment. Figure 1 Š   Context needs to be defined and compiled so that frame conditions, limitations and ambitions for the installation (and its areas and activities) are available for relevant personnel involved in technical safety issues or technical safety management. Examples of context are legislation, standards (internal/ external), concept decisions, operating conditions, prerequisites for use, assumptions/ requirements and NORSOK S-001:018 NORSOK © 018 11 demands to risk reduction. The context applied for the management of technical safety has to be traceable and documented. A major part of the context will be defined early in the development of an installation. During the installation life cycle the context will provide a basis for use/ reassessment and it need to be updated to ensure that all relevant changes and modifications are included.  The starting point for the risk assessment is to identify hazards and their accidental events that are relevant for the design and operation of the installation. Within management of technical safety, various hazard identifications need to be performed. The structure of HAZIDs should preferably be area based, but for some cases they may also be a HAZID node (e.g. part of well, process or utility systems), phase or operational based. Based on hazard identifications it shall be possible to present an overview of possible hazards and accidental events that can occur in different areas and during different activities. The level of detail and depth of hazard identification will be dependent of the maturity of the projects.  Risk and safety analyses / studies shall be performed to establish sufficiently detailed information about the risk associated with the identified hazards and accidental events. The information will be used to evaluate the risk and to decide which solutions (barriers), and related requirements that are needed for preventing, controlling and mitigating the hazards in addition to generic requirements given by the context. Evaluation of risk includes an assessment of: compliance with predefined evaluation criteria (e.g. minimum requirements and acceptance criteria in context); necessary ALARP processes to demonstrate that risk has been reduced to a level as low as reasonably practicable; uncertainties associated with the hazards, accidental events and their consequences as well as the risk reducing effect of the barriers. The results from risk analyses are used for many purposes. One is to provide information and decision support related to the need for and role of risk reducing measures (barriers) and their required performance. Another is to provide decision support regarding the risk level assessed and if this is considered acceptable for the facility. Reference is made to subclause .10 for examples of studies and evaluations. For a development project, the degree of details in the risk and safety analyses / studies will increase as the project matures through different phases. Thus, solutions, assumptions and conservative estimates typically used in early stages may be verified or changed due to more detailed analyses.  The need for barrier functions shall be established based on the context, identified hazards and accidental events, risk analyses and risk evaluation activities.  shall be prepared so that it is possible to identify the need for barrier functions in each installation area or relevant HAZID node. When the need for barrier functions are identified, systems and elements necessary for realizing the barrier functions shall be defined.  Technical barriers often require some form of monitoring, control or activation by people to function as intended. Depending on the characteristics of the facility and its risk picture, different levels of automation may also be chosen for certain safety systems. Therefore, operational and emergency situation considerations shall be an integral part of technical barrier process. As part of project development, safety system design shall include a human factors study amongst others documenting the following: Identification of safety critical tasks (ﬁoperational barrier elementsﬂ) required for the safety system to function. These include tasks related to start-up, monitoring, operation, incident response and recovery in the event of technical failure. Description of performance requirements. These include who is responsible for performing a task, under what circumstances it is expected to be performed, available response time and how it shall be carried out. The results from the study shall be used as input to design, as well as preparations for operations. Input to design should include HMI and alarm system specifications, levels of automation, equipment labelling, system capacities and tolerances. This standard focuses on technical design requirements and addresses operational and organizational aspects supplementing the technical barriers.   shall be prepared to record how specific hazards or accidental events are managed by the use of barrier functions, systems and elements. This documentation can be denoted the 'safety strategy™ (or ‚the barrier strategy™) and can replace the need for Fire and Explosion Strategy (FES) and the Escape, Evacuation and Rescue Strategy (EER strategy) as required by ISO 170.  do not necessarily need to be described in a single document. The strategy may be described and included in other relevant documentation where this is natural and appropriate. The need to develop separate strategies can be viewed in relation to the other documentation which exists or is prepared for the individual facility. Safety strategy documentation should also be prepared to outline applicable overall principles for design, layout, arrangement, philosophies and other high-level design and operational aspects related to barriers; e.g.: how different safety documentation are linked together; risk reduction principles - inherent safety design; premises for design; design provisions for the operating phase; accidental loads and resistance.  Verifiable performance requirements shall be established to ensure that the barrier function is fulfilled. In some situations, performance requirements can also be set directly to barrier functions. Performance requirements shall be established as an integrated part of the design and construction process, as the decisions on what safety systems and barriers to install and their corresponding specifications are made. Performance requirement (PR) for technical barrier elements can be divided into the following categories: Functionality i.e. the ability of the barrier or barrier element to execute the objectives (intended role) affecting the progress of an accident, e.g. by ensuring capacity and effectiveness. The NORSOK S-001:018 NORSOK © 018 1 minimum functional requirement of barrier/barrier element is often given by regulations, referred standards and company internal requirements. However, the specific safety strategy can call for stricter or more nuanced requirements. Integrity of the barrier/barrier element, i.e. the barrier / barrier element™s ability to be present when needed (reliability and availability). These requirements can be determined based on specific safety analysis-/studies or the implementation of generic minimum requirements. The following general requirements apply: o Design and realisation, inclusive of relevant operating issues, of all safety instrumented systems (SIS) shall be based upon the principles of IEC 108/IEC 111. The minimum requirements presented in Norwegian Oil and Gas Association GL070 may be used instead of a full safety analysis/risk assessment for standardised solutions. o The applicable safety system, or affected parts of it, shall be designed to fail-to-safe principle, whereby the system goes to a predefined safe state in the event of detectable malfunction. It shall be designed with the aim of avoiding single defects / failures that may prohibit safety actions being executed. If it is not feasible to implement a fail-to-safe principle, an equivalent level of safety shall be achieved by redundancy and/or diagnostics and fault alarm to relevant manned control room. o The probability of single defects / failures causing inadvertent trip actions shall be as low as reasonably practicable (e.g. provide fault tolerance by means of automatic diagnostic features and redundancy). o All barriers or parts thereof, shall be protected against or withstand environmental conditions that may compromise their safety functions, e.g. ice, snow, sand, water, etc. Survivability of the barrier/barrier element, i.e. its ability to function under relevant accident scenarios and loads. Equipment with a safety function, during and after the accident, should be located so that the possible impact from accidental loads is minimised. To develop the survivability requirements, the design loads that shall form the basis for design of facilities, systems and equipment need to be determined, ref. subclause . Accidental loads and resistance. Barriers/safety systems may be dependent on safety critical tasks to function, through e.g. monitoring, activation or control. For relevant safety systems, performance requirements should also be defined for operational / organizational barrier elements, ref. subclause .. Each clause of this document from clause  and onwards describes generic design principles and requirements for the different safety systems and barriers. The installation specific performance requirements shall be developed based on this framework to manage the risk.  It may be beneficial to group the various performance requirements into performance standards including a description of the role of the safety functions. Dependencies on and interfaces with other systems should also be described.  A Safety Requirement Specification (SRS) is a documentation of requirements related to safety instrumented systems (SIS). The SRS documentation shall be developed during projects and shall provide the design basis for required SIS. ly, the SRS shall contain the relevant key information for use in specifying and operating the instrumented safety functions. However, the information required may be contained in other project documents referred to in the SRS, e.g. performance standards. Duplication of information should be avoided. The SRS shall contain three main types of requirements: NORSOK S-001:018 1 NORSOK © 018 functional requirements such as capacities and response times, integrity requirements such as PFD and SIL, and, operating prerequisites and constraints. Further reference is given to IEC 111 (Functional Safety Œ Safety Instrumented Systems for the process industry sectorﬂ) and Norwegian Oil and Gas Association GL070. .  that needs to be developed to deepen or clarify performance requirements when necessary. Ref. subclause .10 . Also, see Annex C for proposed format and information for data sheets for selected Safety Equipment. .  In concept development, priority shall be given to solutions that are inherently safe. If the hazard cannot be eliminated, probability reducing measures should be given priority over consequence reducing measures. The objectives of risk reduction principles and inherent safety design are to: eliminate or reduce potential hazards/increase inherent safety by; reduction, e.g. reducing the hazardous inventories or the frequency or duration of exposure; substitution, e.g. substituting hazardous materials with less hazardous ones; attenuation (moderation), e.g. using the hazardous materials or processes in a way that limits their hazard potential; simplifications, e.g. making the facility and process simpler to design, build and operate, hence less prone to equipment, control and human failure; reduce probability of hazardous events; establish mitigating measures, e.g. through safety barriers. The ALARP principle (As Low As Reasonable Practicable) shall be used to select the safety solutions. .  Effective management of technical barriers in project development and design processes also need to address relevant dependencies with operational and organizational aspects for the operating phase. Some examples of interfaces between technical, operational and organizational aspects to be considered are: operational prerequisites for start-up and use; measures and restrictions that are necessary in the event of overriding, disconnection or in the event of missing/impaired safety systems and barriers; maintenance; competence; emergency preparedness; manual intervention. In order to ensure solutions which are suited for varying conditions, particular prerequisites shall be accommodated for in the design phase (and sustained during the operating phase). Examples of aspects that should be addressed are: assumptions including conditions and possible actions, when operating in different modes, i.e. normal, test, fault, failure, degraded. (Relevant assumptions in risk analyses should be according to requirements in the different installation specific performance standards); NORSOK S-001:018 NORSOK © 018 1 provisions, routines and logs for isolation of safety related functions during testing and maintenance, e.g. by inhibit (disabling input signal) and override (disabling output action). Such isolation should not render unnecessarily large parts of the system inactive. Logging, manual or automatic, of any such isolation action, e.g. time, number and duration, is mandatory; requirements for compensatory measures. (Responsible personnel for the operating phase will need to implement the necessary measures to remedy or compensate for non-conformities, missing or impaired barriers). The basis for inspection, testing and maintenance shall be described as part of project development in close liaison with the end user and be finalized before start-up. Important elements are: Systems, equipment and barriers shall be classified as regards the health, safety and environment consequences of potential functional failures. Information in performance standards shall regardless of other criticality analyses (e.g. according to NOR</t>
-  </si>
-  <si>
-    <t>7.1 Role</t>
-  </si>
-  <si>
-    <t>7.2 Interfaces</t>
-  </si>
-  <si>
-    <t>7.3 Required utilities</t>
-  </si>
-  <si>
-    <t>7.4 Functional requirements</t>
-  </si>
-  <si>
-    <t>7.5 Survivability requirements</t>
-  </si>
-  <si>
-    <t>8 Containment</t>
-  </si>
-  <si>
-    <t>8.1 Role</t>
-  </si>
-  <si>
-    <t>8.2 Interfaces</t>
-  </si>
-  <si>
-    <t>8.3 Required utilities</t>
-  </si>
-  <si>
-    <t>8.4 Functional requirements</t>
-  </si>
-  <si>
-    <t>8.4.1 General</t>
-  </si>
-  <si>
-    <t>8.4.2 Piping</t>
-  </si>
-  <si>
-    <t>8.4.3 Flanges and connections</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The number of mechanical connections (flanges and hubs) in systems with hydrocarbon inventory shall be kept to a minimum, i.e. by use of welded connections where feasible. Mechanical connections in a hydrocarbon piping system shall as a minimum conform to NORSOK L-001. NOTE It should be noted that flanges of a compact type, according to NORSOK L-00, have a significantly lower leak frequency as compared to traditional ASME flanges. Hence, a reduced risk level can be obtained by selecting compact type flanges. Relief/emergency depressurisation headers should be designed without flanges. Flanges for future tie-ins is acceptable. These shall be of a compact type. Passive fire protection shall be applied in accordance with subclause 0... NORSOK S-001:01 NORSOK © 01 9 There should be no flanges in hydrocarbon piping to, or through, the utility area to avoid hazardous classification and resulting requirements for additional safety systems and barriers. One flanged connection may be installed on the fuel line to each combustion engine, turbine and fired unit in the utility area as well as transfer lines in offloading systems in utility areas for connecting the equipment without affecting the area classification. With respect to instrument connections (connected to a piping valve) to hydrocarbon vessels, piping or equipment, the bore/orifice through the vessel-/piping wall (through nozzle) should be as small as possible to minimise the leak rate in the event of instrument connection leaks. Consideration shall be made to possible hydrate formation, wax deposit or plugging due to other deposits. A flanging philosophy should be established by relevant disciplines, taking into account the installation and operational risk of type of connections and welded solutions. ly, the number of flanges should be minimized. </t>
-  </si>
-  <si>
-    <t>8.4.4 Risers</t>
-  </si>
-  <si>
-    <t>8.5 Survivability requirements</t>
-  </si>
-  <si>
-    <t>9 Open drain</t>
-  </si>
-  <si>
-    <t>9.1 Role</t>
-  </si>
-  <si>
-    <t>9.2 Interfaces</t>
-  </si>
-  <si>
-    <t>9.3 Required utilities</t>
-  </si>
-  <si>
-    <t>9.4 Functional requirements</t>
-  </si>
-  <si>
-    <t>9.4.1 Minimize fire/escalation risk arising from spills and leaks</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Measures shall be provided for dealing with spills and leaks in all areas that have a source of flammable or hazardous liquid so as to minimize the risk of fires and personnel exposure to hazardous materials. The drainage systems shall be designed in accordance with NORSOK P-00 and ISO 10. The capacity of the drainage system, i.e. including overflow lines for fire water, shall be able to handle full fire water capacity and the liquid leak rate associated with the worst credible process fire, typically  kg/s within the bunded area. The drain header capacity shall be sufficient to avoid backpressures that cause liquid to flow back into other open parts of the system during deluge/firefighting. Simultaneous deluge/firefighting in relevant number of areas shall be considered, according to the safety strategy. All tanks and vessels containing flammable liquids shall have a deck bunding covering the tank perimeter controlling spreading of spills, and there shall be drainage within the bunding. Design of the drain system to handle fire water on a floater is challenging due to vessel motions which may result in liquid flowing directly to sea. Particular attention should be made to prevent spreading of fire water and drainage between fire areas, decks and lower escape ways. Tanks collecting drains from hazardous areas shall be purged with inert gas to prevent explosive mixtures. </t>
-  </si>
-  <si>
-    <t>9.4.2 Separation of drain systems</t>
-  </si>
-  <si>
-    <t>9.5 Survivability requirements</t>
-  </si>
-  <si>
-    <t>10 Process safety system</t>
-  </si>
-  <si>
-    <t>10.1 Role</t>
-  </si>
-  <si>
-    <t>10.2 Interfaces</t>
-  </si>
-  <si>
-    <t>10.3 Required utilities</t>
-  </si>
-  <si>
-    <t>10.4 Functional requirements</t>
-  </si>
-  <si>
-    <t>10.4.1 Process safety principles</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The process safety functions shall provide a reliable and fast detection of process upsets and execution of the actions that are considered necessary to control the situation and avoid escalation. For topside functions, the PSD system shall be independent from the process control system. For subsea systems requiring PSD protection, the PSD function shall be independent of the subsea control system, i.e. if any failure of the subsea control system will require PSD protection, e.g overpressure protection. Process and auxiliary systems shall be designed such that no single failure during operations can lead to unacceptable hazardous situations. The process safety system shall normally provide two levels of protection to prevent or minimize the consequences of an undesirable event within the process. If practicable, the two levels shall be provided by functionally different types of device. The design shall be in accordance with NORSOK P-00. Process safety layers of protection shall be established and designed in accordance with API RP 1C or ISO 1 including referenced process standards that in a prescriptive manner often make recommendations of conventional solutions. Note that ISO 1 in subclause ..1 states that if an instrument-based system is used for primary protection, it will not need to comply with IEC 111-1 provided the secondary protection system is self-actuating (PSV or rupture disc) and meets the requirements of relevant codes and standards. Then, a deterministic approach based upon industry accepted typical protective solutions is also acceptable for PSD functions, e.g predefined performance requirement (PFD values) as established in Norwegian Oil and Gas Association GL00. In order to avoid cascading effect, the process shutdown shall be realized in accordance with ISO 1, ..1 / API RP 1C, ... Where utilities, such as cooling water, are shared by process systems and equipment in non-hazardous areas, the utility system shall be designed to prevent migration of flammable liquids and gases into non-hazardous areas and systems. Loss of instrument air or hydraulic supply (PALL) shall initiate a full production shutdown. </t>
-  </si>
-  <si>
-    <t>10.4.2 Process shutdown (PSD) valves</t>
-  </si>
-  <si>
-    <t>10.4.3 Pressure safety valves (PSVs)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> PSVs shall be designed, installed and maintained according to recognized international standards (API STD 0/1). </t>
-  </si>
-  <si>
-    <t>10.4.4 Alarms, automatic actions</t>
-  </si>
-  <si>
-    <t>10.4.5 Response time</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The maximum response time of a process safety function to reach safe state on demand in actual operation shall be defined according to process dynamic behaviour. Typical response times that shall be complied with unless faster responses are required from dynamic analysis: Time from signal from sensor to start of PSD execution, e.g. de-energised solenoid valve, should be less than  seconds. PSD valve travel time (in service) should not exceed  seconds/inch (valve size) to reach safe state. For valves  inch or less, a typical travel time should be set to 1 seconds. New valves should have a design margin to allow for degradation during service life, typically 1 second/inch. </t>
-  </si>
-  <si>
-    <t>10.4.6 Logic solver</t>
-  </si>
-  <si>
-    <t>10.4.7 Instrument based systems for secondary pressure protection</t>
-  </si>
-  <si>
-    <t>10.5 Survivability requirements</t>
-  </si>
-  <si>
-    <t>11 Emergency shutdown (ESD)</t>
-  </si>
-  <si>
-    <t>11.1 Role</t>
-  </si>
-  <si>
-    <t>11.2 Interfaces</t>
-  </si>
-  <si>
-    <t>11.3 Required utilities</t>
-  </si>
-  <si>
-    <t>11.4 Functional requirements</t>
-  </si>
-  <si>
-    <t>11.4.1 Manual ESD activation</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Manual activation of the ESD system shall be possible from strategically positioned stations where accessibility and manning in a hazard situation is taken into account. Possibility for manual activation should be provided at strategic positions such as: CCR (APS/ESD1/ESD); helideck (APS); muster areas/lifeboat stations (APS); bridge connections (ESD); NORSOK S-001:01  NORSOK © 01 drilling areas (driller shutdown and ESD); exits from process and wellhead areas (ESD); strategic located stations along escape routes (ESD). APS activation possibility to be considered at bridge landings in addition to CCR. Manual activation buttons shall be protected against inadvertent activation, e.g. with protective covers or rotary switch and duplicated buttons for APS. Each activation button shall be clearly marked, and a consistent colour coding shall be applied for the activation buttons, e.g. black with yellow stripes for APS and yellow for ESD. Isolation of emergency power supplies i.e. UPS upon APS shall be executed via a timer independent of the logic solver, normally 0 min to ensure that necessary safety critical equipment is in operation during escape and evacuation. Separate function(s) shall be provided allowing bypassing timer based APS countdown. An independent function, e.g. disconnecting the power to the ESD logic solvers, shall be included allowing safe shutdown upon failure of programmable logic. The function may be realized by setting the installation in a safe state, i.e. initiating emergency depressurization and shutdown equivalent to an ESD1 level. Special consideration shall be made to disconnection of centralised escape lights such that no single fault shall result in disconnection of all escape lights. </t>
-  </si>
-  <si>
-    <t>11.4.2 Emergency shutdown (ESD) final elements</t>
-  </si>
-  <si>
-    <t>11.4.3 Emergency shutdown (ESD) actions</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The ESD system shall activate all actions in accordance with the Safety Strategy. Consideration shall be given to interrelations between interconnected installations, e.g. by pipelines or control systems. The ESD functions shall be arranged in a tree-structured hierarchy, APS, ESD1 and ESD.  principles are shown in Figure  and should be used as basis for the facility specific safety strategy. The ESD hierarchy should be simple and unambiguous minimizing number of sub-levels. A higher ESD level shall initiate lower levels including PSD. A signal on a certain level should never initiate shutdowns or actions on higher levels. ESD actions shall include depending on ESD level (see Figure ): shutdown of dry well trees, riser valves and subsea well trees when wells are located within the platform safety zone. NOTE with reference to Figure , shutdown will include closure of DHSV and/or SSIV for specific scenarios; initiate stop of subsea pipeline and flowlines connected to the installation outside of the platform safety zone. The closure signal for both subsea wells and other imports can be realized in subsea control system, except upon APS and F&amp;G detection in riser area where isolation is performed by ESD power cut to subsea facility, ref ... For other imports, the ESD system submits a PSD signal (or by fail to safe PCS signal) to the connected sources (riser valves), ref. subclause ..1; shutdown and sectioning of the hydrocarbon process facilities; initiation of EDP; ignition source isolation; shutdown of main power generation; start/stop of emergency power generator via voltage sensor; shutdown of drilling, intervention and work-over equipment not required for well control. Any shutdown, spurious or intended, shall require a manual reset from CCR. During well intervention DHSV and master valves shall be disconnected from the platform ESD system. It shall be possible to operate the DHSV and master valves in accordance with subclause .. NORSOK S-001:01  NORSOK © 01 Loss of ESD signals between an NNMI and remote control centre shall shutdown the NNMI upon a time delay. The time delay should not exceed  min. ESD of the remote control centre shall result in shutdown of the NNMI. When installed, remotely operated Subsea Isolation Valves (SSIV) shall as a minimum be automatically closed upon APS activation and confirmed fire or gas detection in riser area. The X-mas tree valves part of the ESD function of well stream isolation shall, for subsea installations, apply a fail-to-safe principle for both electrical and hydraulic power supplies. Figure  Š Emergency shutdown (ESD) (principal hierarchy Œ more detailed and other requirements apply) Notes (a) The closure signal for both subsea and other imports can be realized in PCS, except upon F&amp;G detection in riser area where isolation is performed by ESD (power cut to subsea facility, ref ..) or PSD (other imports). (b) Alternative to ESD1 can be ESD and selective electrical isolation disconnection depending on location, e.g. located in close proximity to process, wellhead or drilling areas. (c) Dampers closed/fans stopped on single gas alarm in ventilation intake. (d) The start function shall be inhibited if gas has been detected in air intakes to generator, or generator has previously been tripped due to overspeed. Inhibit start of emergency generator may be also considered due to ISC. For power supplied from subsea cable, the emergency generator only to start upon loss of all cable supplied power. (e) Activation of firefighting systems manually via deluge release pushbutton (not via pressure transmitter feedback, see subclause 1..) shall only initiate ESD and not automatic depressurization. Automatic NORSOK S-001:01 NORSOK © 01  EDP at confirmed gas detection shall be evaluated as a mean to limit extent and duration of possible gas leaks, ref subclause 1... (f) Annunciation (alarm and personnel warning) shall be given together with relevant shutdown level. (g) Immediate shutdown of equipment can be required, see subclause 1... (h) Shutdown of main generator will also include essential generator, if installed (trip both production and drilling). Main power generation until ESD1 premises dual fuel generators. (i) Activation of DHSV and ASV on detection in wellhead area refers to topside wells. Refer to key (a) for subsea wells. (j) Main power switchboard if power is supplied from subsea cable. Emergency board should be operative as long as possible to avoid need for start-up of emergency generator, ref. key (d). (k) For typical emergency consumers in drilling mode, refer to clause 1 and NORSOK D-001. (l) On confirmed gas unless otherwise specified in Safety Strategy (see Clause 1, Table ). (m) With respect to possible ignition sources (Ex equipment), see subclauses 1..1, 1.. and 1... (n) The intention of the LAHH on ESD level is to provide a secondary instrumented process protection level. As an alternative to initiation of ESD, shutdown of relevant ESD valves (using the ESD solenoid valves) and initiation of PSD is acceptable. PSD does not initiate general alarm, stop of fuel gas and ignition source isolation. </t>
-  </si>
-  <si>
-    <t>11.4.4 Emergency shutdown (ESD) alarm annunciation</t>
-  </si>
-  <si>
-    <t>11.4.5 Emergency shutdown (ESD) response time</t>
-  </si>
-  <si>
-    <t>11.4.6 Logic solver</t>
-  </si>
-  <si>
-    <t>11.4.7 Emergency shutdown (ESD) independence</t>
+    <t>5.2 Crane actions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ............................................................................................................................. 10 . </t>
+  </si>
+  <si>
+    <t>5.3 Deck area actions</t>
+  </si>
+  <si>
+    <t>5.4 Tank pressures and tank weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ................................................................................................ 1 . </t>
+  </si>
+  <si>
+    <t>5.4.1 Hydrostatic pressures</t>
+  </si>
+  <si>
+    <t>5.4.2 Ballast</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .................................................................................................................................... 1 . </t>
+  </si>
+  <si>
+    <t>5.5 Variable actions in temporary phases</t>
+  </si>
+  <si>
+    <t>6 Metocean actions</t>
+  </si>
+  <si>
+    <t>6.1 General</t>
+  </si>
+  <si>
+    <t>6.1.1 Metocean data for design and operation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ............................................................................... 1 .1. </t>
+  </si>
+  <si>
+    <t>6.1.2 Possible consequences of climate changes</t>
+  </si>
+  <si>
+    <t>6.1.3 Determination of characteristic metocean actions</t>
+  </si>
+  <si>
+    <t>6.1.3.1 General</t>
+  </si>
+  <si>
+    <t>6.1.3.2 Definition of characteristic actions – ULS and ALS limit states</t>
+  </si>
+  <si>
+    <t>6.1.3.3 Estimation of characteristic actions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> For fixed structures behaving quasi-statically, q-probability hydrodynamic actions can be estimated using the design wave method. See ..1. and ... for further specifications of the design wave method. In particular, if design wave characteristics are established conditionally with respect to directions, corrections suggested in .1. apply. For other structures, q-probability actions and action effects should if possible be based on long-term action or action effect analyses. The resulting annual exceedance probability is estimated by a weighted sum of the contribution from each short-term metocean condition. The weights are the probability of the particular conditions. Two essentially different approaches for the long-term analyses are recommended: Œ all short-term conditions approach; Œ storm event approach. These methods are described in more detail in A.. In addition, the metocean contour method (an approximate method using only short-term analysis) is recommended for nonlinear problems. Metocean contour method If the problem under consideration is of a very nonlinear nature, an extensive model test program may be necessary to model the short-term variability for all important metocean conditions. In particular, this will be the case if the problem is of an on-off nature. For such cases, a simplified and approximate approach may be useful Œ in particular for early phase concept evaluations. A method suggested for this purpose is the metocean contour method. In its present formulation, it is a simplified approach for the all short-term conditions approach. The method is described in more detail in A., but the main steps are listed below: 1) Establish q-probability contours of the metocean characteristics, e.g. significant wave height and spectral peak period. ) Identify the worst metocean condition along the contour for the variable under consideration. ) For this sea state, determine the distribution function for the -hour extreme value for the variable under consideration. ) Estimate the q-probability value from the -percentile of this distribution. For ULS = 0,9 is recommended, while for ALS = 0,9 should be used. The values given above are expected to be slightly conservative if the coefficient of variation does not exceed 0,0 for the -hour extreme value of the variable under consideration. If the coefficient of variation exceeds 0,0, the adequacy of the contour method can be questioned and studies shall be performed in order to establish the appropriate values of . .1. </t>
+  </si>
+  <si>
+    <t>6.1.4 Determination of effects of directional metocean conditions</t>
+  </si>
+  <si>
+    <t>6.2 Modelling of metocean conditions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .............................................................................................. 1 ..1 </t>
+  </si>
+  <si>
+    <t>6.2.1 Wave conditions</t>
+  </si>
+  <si>
+    <t>6.2.1.1 General</t>
+  </si>
+  <si>
+    <t>6.2.1.2 Wave theories</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Irregular sea analyses Provided the action effect under consideration is not sensitive to neither the local wave crest height nor the kinematics close to the crests, use of linear wave theory will most often give sufficient accuracy. This means that a Gaussian wave surface process can be assumed. As far as this is considered accurate, the action effect analyses can conveniently be done in frequency domain, provided structural system is of a linear nature. If the action effect under consideration is sensitive to kinematics close to the wave crests (e.g. drag dominated structures), a second order random process shall be adopted for the surface process. Modelling of the consistent second order surface process and corresponding kinematics are detailed in DNV-RP-C0. For a second order surface process, kinematics based on Wheeler stretching may be applied for early phase design evaluations. For final design Wheeler stretching is not recommended for estimation of extreme hydrodynamic actions of drag dominated structures since this method underestimates the kinematics at still water level Œ in particular for steep waves. A comparison of second order kinematic models, Wheeler stretching and laboratory measurements are shown the commentary section, see ŸA.Ž. Special consideration should be made for crest kinematics in sea states with near breaking waves or breaking waves. Actions on flexible risers and mooring lines attached to large volume floating structures can be calculated based on linear wave theory with due considerations to wave kinematics above SWL and the effect of NORSOK N-00:017 provided by Standard Online AS for DNV GL Group Companies til 00-01-NORSOK N-00:017 NORSOK © 017 17 disturbed kinematics due to large volume wave diffraction. Consistency between floater motions and wave kinematics model used for calculating actions on attached slender structures should be ensured. Regular wave analysis For fixed structure members with cross-sectional dimensions much less than the wavelength (&lt;0,, a regular Stokes th order wave (Fenton, 198) shall be used for ULS and ALS analysis. For floaters linear sinusoidal waves can be used provided the characteristic wave height is calibrated against irregular sea analyses. Water depth limitation The validity of regular wave theories in shallow water is determined by the Ursell number = where H is wave height, k is wave number and d is the water depth. Airy and Stokes wave theory (second-order and higher) is valid if &lt;/ . The same criterion applies to second order random waves where the Ursell number is defined in terms of significant wave height and wave number corresponding to peak spectral period (Stansberg, 011). ..1. </t>
+  </si>
+  <si>
+    <t>6.2.1.3 Regular design waves</t>
+  </si>
+  <si>
+    <t>6.2.1.4 Non-periodic waves</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> As an alternative to periodic regular wave theories, representative waves from a random sea derived with non-periodic wave theories such as ﬁNew-waveﬂ theory may be used. See ISO 19901-1 for further recommendations. ..1. </t>
+  </si>
+  <si>
+    <t>6.2.1.5 Design irregular wave conditions</t>
+  </si>
+  <si>
+    <t>6.2.1.6 Long-term modelling of wave conditions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> All sea state approach A short-term wave condition is characterized by the significant wave height, spectral peak period and mean direction of wave propagation. For an all sea states approach regarding long-term analysis of actions and action effects, the joint distribution of these variables are required. Usually the mean direction of propagation is pooled into a limited number of wave sectors. The long-term distribution of mean direction of wave propagation, , is modelled by a probability mass function, (), estimated directly from data. For each sector, the long-term variablility of wave conditions are described by the joint probability density function of significant wave height, , and spectral peak period, : | (,| )= (|)|(|,) () The following distribution functions are recommended: Œ : A -parameter Weibull distribution. The parameters should be estimated using method of moments. If the frequency of very low sea states ( 1, m) is of main concern, a log Œnormal distribution is expected to give better fit. However, the latter should not be used for &gt;  m. Œ given : A log-normal distribution is generally found to give a good fit with a possible exception for ŸŽ low sea states. For more details on joint distributions of sea state characteristics, reference is made to DNV-RP-C0. Omni-directional modelling is done in a similar way by pooling data from the various direction sectors. 00,0,0,0,811,010100Hs/HsmaxDuration (hours)NORSOK N-00:017 provided by Standard Online AS for DNV GL Group Companies til 00-01-NORSOK N-00:017 0 NORSOK © 017 As the distribution function of significant wave height is available, the q-probability value for is given by the value corresponding to an exceedance probability of , where is the expected number of -hour events per year for the sector under consideration. For an omni-directional analysis, =90. Storm event approach Œ peak over threshold (POT) method If a long-term analysis is to be based on the storm event approach, see Annex A for details, the wave input is time histories of the wave characteristics for all storms exceeding the threshold. Data representing several decades should be available before the storm event approach is utilized for final design. For modelling of long-term variability of storm peaks, a -parameter Weibull model is recommended for storm maximum significant wave height. An alternative model can be the generalized Pareto distribution, but one should be careful if model suggests a too low upper bound for . The conditional distribution of the associated spectral peak period can be modelled by a log-normal distribution. As the distribution function for storm maximum significant wave height is available, the q-probability extreme value is estimated by the value exceeded by the probability /, where is the expected number of storms per year for the sector under consideration. (For an ideal case with data for many decades and with no outliers, the extreme value obtained for the storm event approach is slightly lower than the value obtained for the all sea state approach.) ..1.7 </t>
+  </si>
+  <si>
+    <t>6.2.1.7 Long-term distribution of wave height or wave crest height</t>
+  </si>
+  <si>
+    <t>6.2.2 Current conditions</t>
+  </si>
+  <si>
+    <t>6.2.2.1 General</t>
+  </si>
+  <si>
+    <t>6.2.2.2 Current measurements and design currents</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In most cases a joint occurrence consideration is out of reach. Current conditions at a given location is therefore in most cases characterized by a profile obtained by predicting current speed corresponding to a given annual exceedance probability for each level with a sufficient amount of current measurements. The number of depth levels should be sufficient to capture current phenomena versus depth. As a minimum Œ8 levels seems reasonable depending on water depth ( in upper 0 m, 1 at seabed and the rest equally distributed in between). Prior to establishing current statistics for the purpose of estimating extremes, the deterministic tidal current should be removed from the measurements if it represents a significant part of observed current. The remaining current, the residual part, should be treated statistically. Current extremes at a given depth may be found by fitting a -parameter Weibull model to the residual current. The predicted extreme residual current speed should be added to the tidal current in order to represent design speeds. If current is combined with wind and waves according to Table 7, and wind and waves are dominating the action process, current measurements should be smoothed such that the measurements represents 1-hour average values. -probability events of current can then be taken as the -probability 1-hour current which is assumed to last for the full -hour design weather condition. If current is the governing process, (i.e. ULS case  or ALS case  in Table 7), the -probability current should be taken as the worst 10-minute current during 1/ years. If a simultaneous description of wind, waves and current is used for a long-term response prediction performing analysis for all -hour weather events or selected storm events (POT approach), the default choice should be to use 1-hour current speed assumed to be valid for a -hour period. For such an application there is no reason to remove tidal components. If current show large fluctuations around the 1-hour mean and current is considered very important, one should find ways to account for these fluctuations. A conservative -probability profile for design is obtained by using linear interpolation between -probability values for depths with data. Profiles may be omni-directional or established for the various direction sectors. The profile described above is in most cases conservative due to lack of full correlation between current speeds at different depth levels. If a sufficient amount of data is available Turkstra Models, Winterstein et al. (009) or EOF profiles, Kleiven (00), Forristall and Cooper (1997) may be considered. For early phase design assessments or non-critical marine operations in areas where no accurate measured data or documented numerical studies are available, some guidance is given in A.8. When calculating erosion, it shall be taken into consideration that the structure may change the local current velocity. ... </t>
+  </si>
+  <si>
+    <t>6.2.2.3 Effect on current of adjacent structures</t>
+  </si>
+  <si>
+    <t>6.2.3 Modelling simultaneous occurrence of metocean conditions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ................................................  . </t>
+  </si>
+  <si>
+    <t>6.3 Hydrodynamic actions</t>
+  </si>
+  <si>
+    <t>6.3.1 General</t>
+  </si>
+  <si>
+    <t>6.3.2 Hydrodynamic actions on fixed structures</t>
+  </si>
+  <si>
+    <t>6.3.2.1 General</t>
+  </si>
+  <si>
+    <t>6.3.2.2 Wave and current effect</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Waves and current should be considered when calculating hydrodynamic actions. In combination with waves, the current velocity profile should be stretched to the local water surface. The hydrodynamic action on structural members with a ratio between wavelength () and characteristic dimension () of a member /&gt; should be determined by Morison™s formula using a particle velocity obtained by vector addition of wave and current induced particle velocities. The local normal component of the resulting velocity vector towards the member shall be used in assessing the actions. For large volume structures, with /&lt;, wave diffraction theory should be considered when deriving resultant actions. Wave-current interaction effects should be considered by detailed analysis for e.g.: Œ slowly varying drift forces; Œ air gap; Œ higher order actions; Œ slamming actions. NORSOK N-00:017 provided by Standard Online AS for DNV GL Group Companies til 00-01-NORSOK N-00:017 NORSOK © 017  ... </t>
+  </si>
+  <si>
+    <t>6.3.2.3 Tubular structural elements</t>
+  </si>
+  <si>
+    <t>6.3.2.4 Large volume structures</t>
+  </si>
+  <si>
+    <t>6.3.3 Hydrodynamic actions on floating structures</t>
+  </si>
+  <si>
+    <t>6.3.3.1 General</t>
+  </si>
+  <si>
+    <t>6.3.3.2 Slender structural members</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The formulation of actions in terms of relative velocity is uncertain for facilities with small motion. The method may in such cases give too high damping. Hydrodynamic damping should therefore be taken into consideration through an equivalent viscous damping, and the particle velocity should be used instead of relative motion. Guidance on applicability of relative velocity formulation is given in DNV-RP-C0. When using the relative velocity formulation for structures with large motion in a combined wave and current condition, actions should be obtained for zero as well as maximum current velocity. Depending on whether the drag action is primarily damping or excitation action, low (for damping) and high (for excitation), value of Ÿ Ž should be applied for a conservative estimate of the action. For damping a maximum of 0, is recommended. ... </t>
+  </si>
+  <si>
+    <t>6.3.3.3 Large volume structures</t>
+  </si>
+  <si>
+    <t>6.3.3.4 Freeboard exceedance and green water</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Green water is the overtopping by water of the part of a structure facing the seas in severe wave condition. For a ship, the phenomenon depends on bow shape, design free board, flare, breakwaters and other protective structures, as well as drainage arrangements, and weathervaning procedures. Green water may enter a ship in the bow as well as mid-ship and aft. Significant amounts of green water will have influence on the design of the vessel deck, accommodation superstructure, equipment and layout. It should be noted that for large amounts of green water, the ship motions will also be affected. Freeboard exceedance and green water action effects shall be considered when applicable, see further requirements in 11... ... </t>
+  </si>
+  <si>
+    <t>6.3.3.5 Wave enhancement</t>
+  </si>
+  <si>
+    <t>6.3.3.6 Sloshing actions in tanks</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Motion induced dynamic pressure effects in partially filled tanks, especially with large horizontal dimensions, should be considered. Sloshing represents a dynamic magnification of internal pressure NORSOK N-00:017 provided by Standard Online AS for DNV GL Group Companies til 00-01-NORSOK N-00:017  NORSOK © 017 effects beyond the static pressure. Sloshing occurs if the natural periods of the fluid in tanks and of the vessel motions are close to each other. Possible impact effects should be accounted for in this connection. Sloshing effects depend upon tank dimensions and filling levels, structural arrangement inside the tank and vessel motion characteristics. For design action effects due to sloshing, see NORSOK N-00, L.... .. </t>
+  </si>
+  <si>
+    <t>6.3.4 Hybrid structures</t>
+  </si>
+  <si>
+    <t>6.3.5 Hydrodynamic action for all type of structures</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .......................................................................  . Wind actions ............................................................................................................................... 8 .  .................................................................................................................................. 8 .. Wind conditions ...................................................................................................................... 8 .. Description of wind conditions ............................................................................................... 9 .. Extreme wind speed .............................................................................................................. 0 .. Mean wind actions ................................................................................................................. 0 .. Fluctuating actions .................................................................................................................  ..7 Action effects from wind .........................................................................................................  . Actions from snow ......................................................................................................................  ..1 Action .....................................................................................................................................  .. Mitigations and mitigation effects ...........................................................................................  .. Estimation of snow actions ....................................................................................................  NORSOK N-00:017 provided by Standard Online AS for DNV GL Group Companies til 00-01-NORSOK N-00:017  NORSOK © 017 . Actions from sea spray icing .....................................................................................................  ..1 Actions ...................................................................................................................................  .. Mitigations and mitigation effects ..........................................................................................  .. Marine ice accumulation .......................................................................................................  .7 Actions from atmospheric icing .................................................................................................  .7.1 Actions ...................................................................................................................................  .7. Mitigations and mitigation effects ..........................................................................................  .7. Atmospheric icing accumulation ...........................................................................................  .8 Sea ice actions ..........................................................................................................................  .8.1  ..................................................................................................................................  .8. Actions ...................................................................................................................................  .8. Mitigation and mitigation effects ............................................................................................ 7 .8. Sea ice actions and action effects ........................................................................................ 7 .9 Iceberg actions .......................................................................................................................... 7 .9.1  .................................................................................................................................. 7 .9. Actions ................................................................................................................................... 7 .9. Mitigations and mitigation effects .......................................................................................... 8 .9. Iceberg actions and action effects ........................................................................................ 8 .10 Miscellaneous ............................................................................................................................ 8 .10.1  .................................................................................................................................. 8 .10. Wind chill temperature .......................................................................................................... 9 .10. Frost burst ............................................................................................................................. 9 .11 Other issues related to metocean actions ................................................................................. 9 .11.1 Marine growth and biofouling ................................................................................................ 9 .11. Water level, settlements, subsidence and erosion ............................................................... 0 .11. Appurtenances and equipment ............................................................................................. 0 7 Earthquake actions .............................................................................................................................. 0 7.1 Basis for seismic assessment ................................................................................................... 0 7. Seismic design of structure and foundation .............................................................................. 1 7. Response spectra for a single degree of freedom system ....................................................... 1 8 Deformation actions .............................................................................................................................  8.1  ......................................................................................................................................  8. Temperature actions .................................................................................................................  8. Actions due to fabrication ..........................................................................................................  8. Actions due to settlement of foundations ..................................................................................  9 Accidental actions ................................................................................................................................  9.1  ......................................................................................................................................  9. Fires and explosions .................................................................................................................  9..1  ..................................................................................................................................  9.. Fires ......................................................................................................................................  9.. Explosions .............................................................................................................................  9.. Combined fire and explosion effects .....................................................................................  9. Impact actions ...........................................................................................................................  9..1  ..................................................................................................................................  9.. Vessel collisions ....................................................................................................................  9.. Dropped objects .................................................................................................................... 8 9.. Helicopter impacts ................................................................................................................. 9 9. Effect of subsea gas blow-out ................................................................................................... 9 9. Loss of heading control ............................................................................................................. 9 9. Abnormal variable actions ......................................................................................................... 9 9.7 Failure of DP and stationkeeping .............................................................................................. 0 10 Action combinations ............................................................................................................................ 0 10.1  ...................................................................................................................................... 0 10. Temporary conditions ................................................................................................................ 0 10. Combinations of metocean and earthquake conditions ............................................................  10. Combination of accidental actions ............................................................................................  10.  ..................................................................................................................................  10.. Variable and metocean actions in combination with accidental actions ...............................  NORSOK N-00:017 provided by Standard Online AS for DNV GL Group Companies til 00-01-NORSOK N-00:017 NORSOK © 017  10.. Post damaged condition ........................................................................................................  10. Static and dynamic pressures in tanks ......................................................................................  11 Action effect analyses ..........................................................................................................................  11.1  ......................................................................................................................................  11.1.1 Action effects..........................................................................................................................  11.1. Classification of structures .....................................................................................................  11.1. Classification of analysis types ..............................................................................................  11.1. Determination of characteristic action effects ........................................................................ 7 11.1. Extreme action effects for ultimate limit states (ULS) ............................................................ 8 11.1. Repetitive action effects for fatigue limit states (FLS) ........................................................... 9 11.1.7 Accidental limit states (ALS) analyses ................................................................................... 9 11.1.8 Model testing .......................................................................................................................... 0 11.1.9 Full-scale measurements ....................................................................................................... 1 11.1.10 Modelling of structures by finite element methods................................................................. 1 11. Metocean action effects for structures with only restrained modes ...........................................  11..1 Global analysis .......................................................................................................................  11.. Stochastic wave and current action analysis .........................................................................  11. Rigid body motion analysis for structures with free modes........................................................  11..1 Purpose ..................................................................................................................................  11.. Action processes and operational conditions ........................................................................  11.. Static and mean response analysis .......................................................................................  11.. Dynamic analysis ................................................................................................................... 7 11.. Dynamic system analysis for a short-term period .................................................................. 9 11. Metocean action effects on subsystem structures with free modes .......................................... 70 11. Floater .................................................................................................................................... 70 11.. Mooring and risers ................................................................................................................. 71 11.. Effect of fluid motion in tanks ................................................................................................. 7 11. Topsides ..................................................................................................................................... 7 11..1 Helideck ................................................................................................................................. 7 11. Metocean action effects applicable for all types of structures ................................................... 7 11..1 High frequency action effect analysis .................................................................................... 7 11.. Slamming ............................................................................................................................... 7 11.. Air gap and wave in deck analysis ......................................................................................... 7 11.. Green water ........................................................................................................................... 78 11.. Analysis of action effects due to vortex shedding .................................................................. 78 11.7 Seismic action effects ................................................................................................................ 79 11.7.1  .................................................................................................................................. 79 11.7. Action effects by response spectrum approach ..................................................................... 79 11.7. Global nonlinear strength analysis ......................................................................................... 80 Annex A (informative) Commentary ............................................................................................................ 81 Annex B (informative) Wind chill temperature ........................................................................................... 10 Annex C (informativ) Maximum and minimum air temperature on the Norwegian Continental shelf ...... 11 Bibliography ............................................................................................................................................... 11 NORSOK N-00:017 provided by Standard Online AS for DNV GL Group Companies til 00-01-NORSOK N-00:017  NORSOK © 017 Foreword NORSOK N-00:017, was adopted as NORSOK Standard in January 017. ŸCorrigendum NORSOK N-00:017/AC:018 (indicated in the text by tags ŸŽ) was incorporated into NORSOK N-00:01 in May 018. Ž NORSOK N-00:017, replaces NORSOK N-00, rev. , September 007. NORSOK is an acronym for the competitive position of the Norwegian continental shelf and comprise petroleum industry standards in Norway. The collaboration initiative in 199 between the authorities and the petroleum industry initiated the development of NORSOK standards. Reducing the project execution time and developing and operating cost for petroleum installations on the Norwegian shelf was the target. The intention for the Petroleum industry is to develop and use standards providing good technical and cost effective solutions to ensure that the petroleum resources are exploited and managed in the best possible way by the industry and the authorities. The industry will actively contribute to the development and use of international standards in the global market. The NORSOK standards shall: Œ bridge the gap based on experiences from the Norwegian continental shelf where the international standards are unsatisfactorily; Œ replace oil company specifications where possible; Œ be available as references for the authorities™ regulations; Œ be cost effective; Œ promote the Norwegian sector as an attractive area for investments and activities. Developing new NORSOK standards and regular maintenance of existing standards shall contribute to maintain the competitiveness both nationally and internationally for the Norwegian petroleum industry. The NORSOK standards are developed by experts from the Norwegian petroleum industry and approved according to the consensus principles as laid down by the guidelines given in this NORSOK directive. The NORSOK standards are owned by the Norwegian Oil and Gas Association, the Federation of Norwegian Industries and the Norwegian Shipowners´ Association. They are managed and published by Standards Norway. The principal standard for offshore structures is NORSOK N-001, Structural design, which refers to ISO 19900, Petroleum and natural gas industries Œ  requirements for offshore structures. Main changes in this edition compared to Edition  are: Œ The inclusion of more complete description of cold climate actions from sea ice, icebergs, icing and snow. Œ Updates of accidental actions due to ship collision risk. Œ The standard now allows the use of hindcast data as basis for design. Œ Air gap recommendations included. Œ Adjustments are made to the recipe for wave action effects on jacket structures, including wave kinematics and wave crest. Œ The standard now allows for the use of CFD methods in wave load calculation. Œ Wave impacts actions are updated to include impacts from breaking waves, slamming on vertical structures, and wave impact in floater deck. Œ Action combinations are updated e.g. to include cold climate actions in ULS and ALS. ALS in damaged condition is updated for actions uncorrelated with the accidental event. Œ Sections on design waves, contour method, and long-term analysis are rewritten and updated according to present knowledge. Œ The inclusion of a section on climate change. Œ The preparation for the removal of NORSOK N-00 Collection of Metocean Data has resulted in the inclusion of some issues into this standard, e.g. recommended duration of metocean measurements. The major part of NORSOK N-00 is found in ISO 19901-1 Metocean Design. NORSOK N-00:017 provided by Standard Online AS for DNV GL Group Companies til 00-01-NORSOK N-00:017 NORSOK © 017  Œ The informative Annexes A, B and C are new. NORSOK N-00:017 provided by Standard Online AS for DNV GL Group Companies til 00-01-NORSOK N-00:017  NORSOK © 017  This NORSOK standard specifies general principles and guidelines for determination of characteristic actions and action effects for design, assessment and verification of structures. Reference is made to NORSOK N-001 (and NORSOK N-00) as to how this standard is to be used to achieve the desired safety level for new and existing structures. This NORSOK standard is applicable to all types of offshore structures used in the petroleum activities, including bottom-founded structures as well as floating structures, including substructures, topside structures, vessel hulls, foundations, mooring systems, risers and subsea facilities. This NORSOK standard is primarily written for the design of new facilities on the Norwegian continental shelf (including the continental shelf of Svalbard) as defined by NPD 1.0.01, but the principles may also be applicable for other areas.  The following standards include provisions and guidelines which, through reference in this text, constitute provisions and guidelines of this NORSOK standard. Latest issue of the references shall be used unless otherwise agreed. Other recognized standards may be used provided it can be shown that they meet the requirements of the referenced standards. DNVGL-OS-C101, Design of offshore steel structures, general Œ LRFD method, Ch., Sec. .. Tank pressures (Ed 01). NORSOK N-001, Integrity of offshore structures FOR-007-10--1181, Forskrift om kontinentalsokkelflyging - ervervsmessig luftfart til og fra helikopterdekk på innretninger og fartøy til havs   .1  .1.1 action assembly of concentrated or distributed forces acting on a structure (direct actions), displacements or thermal effects imposed to the structure, or constrained in it, or environmental influences that may cause changes with time in the material properties or in the dimension of a structure (ISO 9) .1. action effect effects of actions (or action effects) is a result of action on a structural member (e.g. internal force, moment, stress, strain) or on the whole structure (e.g. deflection, rotation) (ISO 9) .1. air gap vertical distances measured from still water level (still water air gap) or top of wave crest (air gap) to bottom of steel of deck structure. .1. can Ÿexpression in the content of a document conveying expected or conceivable material, physical or causal outcome. Note 1 to entry: Possibility and capability is expressed using the verbal forms specified in Table . Ž .1. characteristic value value specified preferably on statistical bases, so it can be considered to have a prescribed probability of not being exceeded (ISO 9) NORSOK N-00:017 provided by Standard Online AS for DNV GL Group Companies til 00-01-NORSOK N-00:017 NORSOK © 017 7 .1. design (value of an) action value of an action used in semi-probabilistic verification calibrated to the reliability target. In the partial factor method, the value is obtained by multiplying the representative (characteristic) value by the partial factor (ISO 9) .1.7 design premises set of project specific design data and functional requirements which are not specified or are left open in the general standard .1.8 epistemic uncertainty uncertainties originating from lack of knowledge and understanding of the problem under consideration. Epistemic uncertainties can be reduced by e.g. collection of more data or further investigation regarding statistical models and action models .1.9 freeboard vertical distances measured from still water level to main deck .1.10 inherent uncertainty aleatory or inherent variability (randomness in nature) typically associated with the metocean parameters, the geometry of the structure, and the material properties .1.11 may (permission) expression in the content of a document conveying consent or liberty (or opportunity) to do something Note 1 to entry Permissions are expressed using the verbal forms specified in ISO/IEC Directives Part  clause 7. Table . .1.1 metocean meteorological and oceanographic conditions (including sea ice, icebergs and icing for cold climate areas) for the determination of actions and action effects for the design, construction and operation of offshore structures. Metocean actions are one type of environmental actions .1.1 most probable maximum value of the maximum of a variable with the highest probability of occurring Ÿwithin a specified temporal period or spatial areaŽ .1.1 q-probability annual probability of exceedance equal to q. For q less than 0,1 this corresponds approximately to a return period of 1/q years .1.1 sea state condition of the sea during a period in which its statistical parameters are assumed to remain constant, see stationary condition .1.1 stationary condition the duration of a stationary metocean event is  hours unless stated otherwise NORSOK N-00:017 provided by Standard Online AS for DNV GL Group Companies til 00-01-NORSOK N-00:017 8 NORSOK © 017 .1.17 shall (requirement) expression in the content of a document conveying objectively verifiable criteria to be fulfilled and from which no deviation is permitted if compliance with the document is to be claimed ŸNote 1 to entry: Requirements are expressed using the verbal forms specified in ISO/IEC Directives, Part  clause 7. Table .Ž .1.18 should (recommendation) expression in the content of a document conveying Ÿa suggested possible choice or course of action deemed to be particularly suitable without necessarily mentioning or excluding others Note 1 to entry: Recommendations are expressed using the verbal forms specified in ISO/IEC Directives, Part  clause 7. Table . Note  to entry: In the negative form, a recommendation is the expression that a suggested possible choice or course of action is not preferred but it is not prohibited. Ž .1.19 slender members or slender structures (geometrically) structural members that are geometrically slender, i.e. the length to cross-sectional dimension ratio is large Note 1 to entry: Slender members and slender structures are used in a variety of meanings, e.g. for determining the use of the drag term in the Morison formula. In this standard slenderness is, as the definition states, only used for geometrically slenderness. .1.0 target extreme value extreme value corresponding to an annual probability of exceedance equal to q. For q less than 0,1 this corresponds approximately to a return period of 1/q years .1.1 verification examination to confirm that an activity, a product or a service is in accordance with specified requirements .1. water level mean water level (MWL): arithmetic mean of all sea levels measured over a long period highest astronomical tide (HAT): level of high tide when all harmonic components causing the tides are in phase lowest astronomical tide (LAT): level of low tide when all harmonic components causing the tides are in phase still water level (SWL): abstract water level used in the calculation of elevations at which actions are applied, normally the highest possible water level in extreme weather (see Figure 1). If a low water level is governing (e.g. TLP tendons in slack), LAT can be taken as the still water level (SWL) in extreme weather conditions. In good weather, a water level lower than LAT is possible due to a negative storm surge caused by very high air pressure. NORSOK N-00:017 provided by Standard Online AS for DNV GL Group Companies til 00-01-NORSOK N-00:017 NORSOK © 017 9 Figure 1 Œ Still water level .  ALS accidental limit states CQC complete quadratic combination DAF dynamic amplification factor DP dynamic positioning EOF empirical orthogonal functions FE finite element FLS fatigue limit states FPSO floating production storage and offloading unit GBS gravity based structure HAT highest astronomical tide HF high frequency (higher than wave frequency) ISO International Organization for Standardization KC Keulegan-Carpenter number LF low frequency (lower than wave frequency) MWL mean water level NMA Norwegian Maritime Authority (Sjøfartsdirektoratet) NFR Norges Forskningsråd (The Research Council of Norway) NS Norsk Standard (Norwegian Standard) OTM overturning moment P- effect second order effect of an axial force (P) due to a lateral displacement, POT peak-over-threshold SLS serviceability limit states SRSS square root of sum of squares SWL still water level TLP tension leg platform ULS ultimate limit states VIV vortex induced vibrations WCT wind chill temperature WF wave frequency NORSOK N-00:017 provided by Standard Online AS for DNV GL Group Companies til 00-01-NORSOK N-00:017 10 NORSOK © 017      are actions that will not vary in magnitude, position or direction during the time period considered. Examples are: a) weight of the structure; b) weight of permanent ballast and equipment, including mooring systems and risers; c) external hydrostatic pressure up to the mean water level; d) pretension (static tension in initial position). Characteristic permanent actions are defined by the expected value. .  Structural components subjected to high counteracting hydrostatic pressures, e.g. external walls in fixed concrete structures with in the order of 100 m and higher differential water pressure height, should be designed taking into account the possible uncertainties due to possible variation in: Œ level and density; Œ dimension tolerances; Œ measuring inaccuracies; and other uncertainties affecting the pressure difference. Unless documented otherwise by detailed analyses of operations, the minimum pressure difference for the ultimate limit states should be at least equal to the smallest of one tenth of the maximum pressure and 0,1 MPa.  Variable functional actions .1  Variable actions originate from normal operation of the structure and vary in position, magnitude and direction during the period considered. They include ŸactionsŽ from a) persons, b) helicopters, c) lifeboats, d) cranes, e) tank pressures and weights, f) stored goods, g) modules and structural parts that can be removed, h) weight, pressure and temperature of gas and liquid in process plants, i) local pressure and global effect of variable ballast, j) installation and drilling operations. Assumptions regarding variable actions shall be reflected in the operational manual, and complied with in operation. Possible deviations from the assumed value due to operational errors or mechanical failures or damages shall be treated as accidental actions, see Clause 9. Characteristic values of variable functional actions are defined as a specified value not to be exceeded. .   shall be determined with due account of dynamic effects of crane and, if applicable, the motions of the facility. Fatigue calculations shall be carried out based on expected frequency of crane usage, the magnitude of actions, dynamic effects from wind, loading and discharging of ships and, if applicable, from motions of the facility. NORSOK N-00:017 provided by Standard Online AS for DNV GL Group Companies til 00-01-NORSOK N-00:017 NORSOK © 017 11 .  Variable actions on deck areas of the topside structure shall be stated in the design premises and reflected in the structural load plan drawing or the operational manual and shall be complied with in operation. Variable actions on deck areas of the topside shall as a minimum be based on Table 1 unless larger actions are specified in the design premises. The distributed actions are set to depend on local/global aspects of the deck structure to take into account the spatial variability of the actions (e.g. local peaks in lay-down area need to be accounted for in local design, but can be distributed for design of primary steel). The following notations are used: Local design: design of deck plates, stiffeners and local effects on deck beams and columns; Primary design: design of deck beams, beam-columns and complete modules; Global design: design of global loadbearing structure such as topside main structure, substructure and foundation (e.g. jacket, hull, piles, mooring and anchors). Table 1 Œ Minimum variable actions in deck areas Area Local structure design See 1,, and  Primary structure design Global structure design See  Distribution action, (kN/m) Point action, (kN) Apply factor given below to distributed action, ( = the action area in m) Apply factor given below to distributed action, Storage areas, See  1,· 1,0 1,0 Laydown areas, See  1,· min(1,0;(0, + /0,)) min(1,0; (0. + /0,)) Lifeboat platforms 9,0 9,0 1,0 may be ignored Area between equipment ,0 ,0 min(1,0; (0, + /0,)) may be ignored Walkways, staircases and platforms, crew spaces ,0 ,0 min(1,0; (0, + /0,)) may be ignored Walkways and stair-cases for inspection and repair only ,0 ,0 min(1,0; (0, + /0,)) may be ignored Areas not exposed to other functional actions , , 1,0 may be ignored Roofs, accessible for inspection and repair only 1,0 ,0 1,0 may be ignored 1. Wheel actions to be added to distributed actions, where relevant. Wheel actions can normally be considered acting on an area of 00 mm x 00 mm. . Point actions to be applied on an area 100 mm x 100 mm, and at the most severe position, but not added to wheel actions or distributed actions. . pd is to be evaluated for each case. Storage areas for cement, wet or dry mud should be the maximum of 1 kN/m and gH, where H is the storage heig</t>
+  </si>
+  <si>
+    <t>6.3.5.1 Effect of adjacent structure</t>
+  </si>
+  <si>
+    <t>6.3.5.2 Nonlinear wave actions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Higher order potential flow wave diffraction methods as applicable for large volume structures and nonlinear finite amplitude wave kinematics used in conjunction with Morison™s formula on slender structures, cause mean, sum-frequency and difference frequency actions in irregular waves. Such actions may cause significant response, and hence action effects, if resonance occurs. The higher order actions should be determined by a consistent theory relevant for the structure considered and validated by model tests. Difference (low) frequency wave actions associated with nonlinear wave-body interaction may excite lightly damped resonant modes of motion with natural frequency below the wave frequency range. This may be important for the rigid body motions of floaters and their positioning systems. Both horizontal and vertical modes of motion may be excited. Such motions are also referred to as slowly varying drift motions. Special attention should be paid to wave-current interaction effects and viscous effects on the low frequency wave actions. Due to the uncertainty associated with calculations of slowly varying drift motions model tests are required to reduce the uncertainty when the response is significant. Special care should be taken as the damping may be over-estimated in model tests due to scale effects. Dynamic calculations should be done for both ŸŽ model scale and full scale in order to estimate the scale effect. Sum (high) frequency wave actions may be important for the response of GBS structures and jack-ups in their elastic modes with natural frequencies above the wave frequency range, for tension-leg platforms in their restrained modes and for ship shaped structures in their elastic modes. Sum frequency actions may cause springing response, which may be of importance especially for the fatigue limit states. Actions from steep, high waves on structures extending above the still water level may cause nonlinear transient actions. Structural responses to these actions may be dynamically amplified and cause substantially increased response. Such response is also referred to as ringing. Nonlinear transient actions may be important for structures consisting of large diameter shafts and having a natural period under 8 sec. Actions causing ringing can be estimated by nonlinear potential theory or Computational Fluid Dynamics. One method that predicts ringing actions reasonably well, is presented by Johannessen NORSOK N-00:017 provided by Standard Online AS for DNV GL Group Companies til 00-01-NORSOK N-00:017 NORSOK © 017 7 (011). However, available analysis methods are generally only amenable to screening analysis of the ringing problem. The phenomenon is best quantified by model tests. Actions from wave impact/slamming from steep or breaking waves on GBS structures or waves impacting jacket topside may cause dynamically amplified resonant response. It is then generally difficult to distinguish impact/slamming from higher order wave diffraction effects. With regard to structures that have been optimised with respect to minimal linear wave actions, experience has shown that nonlinear effects may be dominant. Motion analyses for new types of structures where the results cannot be checked against previous experience, should be checked against model tests. ... </t>
+  </si>
+  <si>
+    <t>6.3.5.3 Wave slamming</t>
+  </si>
+  <si>
+    <t>6.4 Wind actions</t>
+  </si>
+  <si>
+    <t>6.4.1 General</t>
+  </si>
+  <si>
+    <t>6.4.2 Wind conditions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ...................................................................................................................... 8 .. </t>
+  </si>
+  <si>
+    <t>6.4.3 Description of wind conditions</t>
+  </si>
+  <si>
+    <t>6.4.4 Extreme wind speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .............................................................................................................. 0 .. </t>
+  </si>
+  <si>
+    <t>6.4.5 Mean wind actions</t>
+  </si>
+  <si>
+    <t>6.4.6 Fluctuating actions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .................................................................................................................  ..7 </t>
+  </si>
+  <si>
+    <t>6.4.7 Action effects from wind</t>
+  </si>
+  <si>
+    <t>6.5 Actions from snow</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ......................................................................................................................  ..1 </t>
+  </si>
+  <si>
+    <t>6.5.1 Action</t>
+  </si>
+  <si>
+    <t>6.5.2 Mitigations and mitigation effects</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ...........................................................................................  .. </t>
+  </si>
+  <si>
+    <t>6.5.3 Estimation of snow actions</t>
+  </si>
+  <si>
+    <t>6.6 Actions from sea spray icing</t>
+  </si>
+  <si>
+    <t>6.6.1 Actions</t>
+  </si>
+  <si>
+    <t>6.6.2 Mitigations and mitigation effects</t>
+  </si>
+  <si>
+    <t>6.6.3 Marine ice accumulation</t>
+  </si>
+  <si>
+    <t>6.7 Actions from atmospheric icing</t>
+  </si>
+  <si>
+    <t>6.7.1 Actions</t>
+  </si>
+  <si>
+    <t>6.7.2 Mitigations and mitigation effects</t>
+  </si>
+  <si>
+    <t>6.7.3 Atmospheric icing accumulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ...........................................................................................  .8 </t>
+  </si>
+  <si>
+    <t>6.8 Sea ice actions</t>
+  </si>
+  <si>
+    <t>6.8.1 General</t>
+  </si>
+  <si>
+    <t>6.8.2 Actions</t>
+  </si>
+  <si>
+    <t>6.8.3 Mitigation and mitigation effects</t>
+  </si>
+  <si>
+    <t>6.8.4 Sea ice actions and action effects</t>
+  </si>
+  <si>
+    <t>6.9 Iceberg actions</t>
+  </si>
+  <si>
+    <t>6.9.1 General</t>
+  </si>
+  <si>
+    <t>6.9.2 Actions</t>
+  </si>
+  <si>
+    <t>6.9.3 Mitigations and mitigation effects</t>
+  </si>
+  <si>
+    <t>6.9.4 Iceberg actions and action effects</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ........................................................................................ 8 .10 </t>
+  </si>
+  <si>
+    <t>6.10 Miscellaneous</t>
+  </si>
+  <si>
+    <t>6.10.1 General</t>
+  </si>
+  <si>
+    <t>6.10.2 Wind chill temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .......................................................................................................... 9 .10. </t>
+  </si>
+  <si>
+    <t>6.10.3 Frost burst</t>
+  </si>
+  <si>
+    <t>6.11 Other issues related to metocean actions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ................................................................................. 9 .11.1 </t>
+  </si>
+  <si>
+    <t>6.11.1 Marine growth and biofouling</t>
+  </si>
+  <si>
+    <t>6.11.2 Water level, settlements, subsidence and erosion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ............................................................... 0 .11. </t>
+  </si>
+  <si>
+    <t>6.11.3 Appurtenances and equipment</t>
+  </si>
+  <si>
+    <t>7 Earthquake actions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .............................................................................................................................. 0 .1 </t>
+  </si>
+  <si>
+    <t>7.1 Basis for seismic assessment</t>
+  </si>
+  <si>
+    <t>7.2 Seismic design of structure and foundation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .............................................................................. 1 . </t>
+  </si>
+  <si>
+    <t>7.3 Response spectra for a single degree of freedom system</t>
   </si>
 </sst>
 </file>
@@ -764,7 +776,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B338"/>
+  <dimension ref="A1:B334"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -787,39 +799,42 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -827,24 +842,18 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1">
@@ -855,6 +864,9 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1">
@@ -876,56 +888,53 @@
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1">
@@ -936,6 +945,9 @@
       <c r="A25" s="1">
         <v>23</v>
       </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1">
@@ -946,24 +958,18 @@
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -986,7 +992,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -994,7 +1000,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1002,7 +1008,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1025,7 +1031,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1033,7 +1039,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1041,7 +1047,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1064,7 +1070,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1072,7 +1078,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1080,7 +1086,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1103,24 +1109,18 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
-      <c r="B52" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
-      <c r="B53" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="1">
@@ -1131,6 +1131,9 @@
       <c r="A55" s="1">
         <v>53</v>
       </c>
+      <c r="B55" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="1">
@@ -1141,35 +1144,35 @@
       <c r="A57" s="1">
         <v>55</v>
       </c>
-      <c r="B57" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
-      <c r="B58" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
+      <c r="B60" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="1">
         <v>59</v>
       </c>
+      <c r="B61" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="1">
@@ -1180,9 +1183,6 @@
       <c r="A63" s="1">
         <v>61</v>
       </c>
-      <c r="B63" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="1">
@@ -1193,6 +1193,9 @@
       <c r="A65" s="1">
         <v>63</v>
       </c>
+      <c r="B65" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="1">
@@ -1203,9 +1206,6 @@
       <c r="A67" s="1">
         <v>65</v>
       </c>
-      <c r="B67" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="1">
@@ -1216,6 +1216,9 @@
       <c r="A69" s="1">
         <v>67</v>
       </c>
+      <c r="B69" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="1">
@@ -1226,24 +1229,18 @@
       <c r="A71" s="1">
         <v>69</v>
       </c>
-      <c r="B71" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="1">
         <v>70</v>
       </c>
-      <c r="B72" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="1">
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1266,18 +1263,24 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="1">
         <v>76</v>
       </c>
+      <c r="B78" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="1">
         <v>77</v>
       </c>
+      <c r="B79" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="1">
@@ -1288,35 +1291,35 @@
       <c r="A81" s="1">
         <v>79</v>
       </c>
-      <c r="B81" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="1">
         <v>80</v>
       </c>
-      <c r="B82" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="1">
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="1">
         <v>82</v>
       </c>
+      <c r="B84" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="1">
         <v>83</v>
       </c>
+      <c r="B85" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="1">
@@ -1327,9 +1330,6 @@
       <c r="A87" s="1">
         <v>85</v>
       </c>
-      <c r="B87" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="1">
@@ -1340,6 +1340,9 @@
       <c r="A89" s="1">
         <v>87</v>
       </c>
+      <c r="B89" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="1">
@@ -1350,9 +1353,6 @@
       <c r="A91" s="1">
         <v>89</v>
       </c>
-      <c r="B91" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="1">
@@ -1363,35 +1363,35 @@
       <c r="A93" s="1">
         <v>91</v>
       </c>
+      <c r="B93" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="1">
         <v>92</v>
       </c>
+      <c r="B94" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="1">
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="1">
         <v>94</v>
       </c>
-      <c r="B96" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="1">
         <v>95</v>
       </c>
-      <c r="B97" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="1">
@@ -1402,35 +1402,35 @@
       <c r="A99" s="1">
         <v>97</v>
       </c>
+      <c r="B99" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="1">
         <v>98</v>
       </c>
+      <c r="B100" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="1">
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" s="1">
         <v>100</v>
       </c>
-      <c r="B102" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="1">
         <v>101</v>
       </c>
-      <c r="B103" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="1">
@@ -1441,35 +1441,35 @@
       <c r="A105" s="1">
         <v>103</v>
       </c>
+      <c r="B105" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="1">
         <v>104</v>
       </c>
+      <c r="B106" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="1">
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="1">
         <v>106</v>
       </c>
-      <c r="B108" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="1">
         <v>107</v>
       </c>
-      <c r="B109" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="1">
@@ -1480,6 +1480,9 @@
       <c r="A111" s="1">
         <v>109</v>
       </c>
+      <c r="B111" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="1">
@@ -1490,24 +1493,18 @@
       <c r="A113" s="1">
         <v>111</v>
       </c>
-      <c r="B113" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" s="1">
         <v>112</v>
       </c>
-      <c r="B114" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" s="1">
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1530,7 +1527,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1538,7 +1535,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1546,7 +1543,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -1569,7 +1566,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1577,7 +1574,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1585,7 +1582,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1608,24 +1605,18 @@
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" s="1">
         <v>130</v>
       </c>
-      <c r="B132" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="1">
         <v>131</v>
       </c>
-      <c r="B133" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" s="1">
@@ -1636,6 +1627,9 @@
       <c r="A135" s="1">
         <v>133</v>
       </c>
+      <c r="B135" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="1">
@@ -1646,24 +1640,18 @@
       <c r="A137" s="1">
         <v>135</v>
       </c>
-      <c r="B137" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="1">
         <v>136</v>
       </c>
-      <c r="B138" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" s="1">
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -1686,7 +1674,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -1694,7 +1682,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -1702,7 +1690,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -1725,24 +1713,18 @@
         <v>147</v>
       </c>
       <c r="B149" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" s="1">
         <v>148</v>
       </c>
-      <c r="B150" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" s="1">
         <v>149</v>
       </c>
-      <c r="B151" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="1">
@@ -1753,6 +1735,9 @@
       <c r="A153" s="1">
         <v>151</v>
       </c>
+      <c r="B153" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" s="1">
@@ -1763,24 +1748,18 @@
       <c r="A155" s="1">
         <v>153</v>
       </c>
-      <c r="B155" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" s="1">
         <v>154</v>
       </c>
-      <c r="B156" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" s="1">
         <v>155</v>
       </c>
       <c r="B157" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -1797,27 +1776,30 @@
       <c r="A160" s="1">
         <v>158</v>
       </c>
-      <c r="B160" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" s="1">
         <v>159</v>
       </c>
       <c r="B161" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" s="1">
         <v>160</v>
       </c>
+      <c r="B162" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" s="1">
         <v>161</v>
       </c>
+      <c r="B163" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" s="1">
@@ -1828,9 +1810,6 @@
       <c r="A165" s="1">
         <v>163</v>
       </c>
-      <c r="B165" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" s="1">
@@ -1841,18 +1820,24 @@
       <c r="A167" s="1">
         <v>165</v>
       </c>
+      <c r="B167" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" s="1">
         <v>166</v>
       </c>
+      <c r="B168" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" s="1">
         <v>167</v>
       </c>
       <c r="B169" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -1875,18 +1860,24 @@
         <v>171</v>
       </c>
       <c r="B173" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" s="1">
         <v>172</v>
       </c>
+      <c r="B174" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" s="1">
         <v>173</v>
       </c>
+      <c r="B175" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" s="1">
@@ -1897,9 +1888,6 @@
       <c r="A177" s="1">
         <v>175</v>
       </c>
-      <c r="B177" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" s="1">
@@ -1910,18 +1898,24 @@
       <c r="A179" s="1">
         <v>177</v>
       </c>
+      <c r="B179" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" s="1">
         <v>178</v>
       </c>
+      <c r="B180" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" s="1">
         <v>179</v>
       </c>
       <c r="B181" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -1944,18 +1938,24 @@
         <v>183</v>
       </c>
       <c r="B185" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" s="1">
         <v>184</v>
       </c>
+      <c r="B186" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" s="1">
         <v>185</v>
       </c>
+      <c r="B187" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" s="1">
@@ -1966,9 +1966,6 @@
       <c r="A189" s="1">
         <v>187</v>
       </c>
-      <c r="B189" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" s="1">
@@ -1979,6 +1976,9 @@
       <c r="A191" s="1">
         <v>189</v>
       </c>
+      <c r="B191" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" s="1">
@@ -1989,9 +1989,6 @@
       <c r="A193" s="1">
         <v>191</v>
       </c>
-      <c r="B193" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" s="1">
@@ -2002,6 +1999,9 @@
       <c r="A195" s="1">
         <v>193</v>
       </c>
+      <c r="B195" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" s="1">
@@ -2012,9 +2012,6 @@
       <c r="A197" s="1">
         <v>195</v>
       </c>
-      <c r="B197" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" s="1">
@@ -2025,18 +2022,24 @@
       <c r="A199" s="1">
         <v>197</v>
       </c>
+      <c r="B199" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" s="1">
         <v>198</v>
       </c>
+      <c r="B200" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" s="1">
         <v>199</v>
       </c>
       <c r="B201" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -2059,18 +2062,24 @@
         <v>203</v>
       </c>
       <c r="B205" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" s="1">
         <v>204</v>
       </c>
+      <c r="B206" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" s="1">
         <v>205</v>
       </c>
+      <c r="B207" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" s="1">
@@ -2081,35 +2090,35 @@
       <c r="A209" s="1">
         <v>207</v>
       </c>
-      <c r="B209" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210" s="1">
         <v>208</v>
       </c>
-      <c r="B210" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211" s="1">
         <v>209</v>
       </c>
       <c r="B211" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212" s="1">
         <v>210</v>
       </c>
+      <c r="B212" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213" s="1">
         <v>211</v>
       </c>
+      <c r="B213" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="214" spans="1:2">
       <c r="A214" s="1">
@@ -2120,9 +2129,6 @@
       <c r="A215" s="1">
         <v>213</v>
       </c>
-      <c r="B215" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216" s="1">
@@ -2133,18 +2139,24 @@
       <c r="A217" s="1">
         <v>215</v>
       </c>
+      <c r="B217" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="218" spans="1:2">
       <c r="A218" s="1">
         <v>216</v>
       </c>
+      <c r="B218" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="219" spans="1:2">
       <c r="A219" s="1">
         <v>217</v>
       </c>
       <c r="B219" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="220" spans="1:2">
@@ -2167,18 +2179,24 @@
         <v>221</v>
       </c>
       <c r="B223" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="224" spans="1:2">
       <c r="A224" s="1">
         <v>222</v>
       </c>
+      <c r="B224" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225" s="1">
         <v>223</v>
       </c>
+      <c r="B225" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226" s="1">
@@ -2189,9 +2207,6 @@
       <c r="A227" s="1">
         <v>225</v>
       </c>
-      <c r="B227" t="s">
-        <v>94</v>
-      </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228" s="1">
@@ -2202,6 +2217,9 @@
       <c r="A229" s="1">
         <v>227</v>
       </c>
+      <c r="B229" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="230" spans="1:2">
       <c r="A230" s="1">
@@ -2212,9 +2230,6 @@
       <c r="A231" s="1">
         <v>229</v>
       </c>
-      <c r="B231" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="232" spans="1:2">
       <c r="A232" s="1">
@@ -2225,6 +2240,9 @@
       <c r="A233" s="1">
         <v>231</v>
       </c>
+      <c r="B233" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234" s="1">
@@ -2235,9 +2253,6 @@
       <c r="A235" s="1">
         <v>233</v>
       </c>
-      <c r="B235" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="236" spans="1:2">
       <c r="A236" s="1">
@@ -2248,6 +2263,9 @@
       <c r="A237" s="1">
         <v>235</v>
       </c>
+      <c r="B237" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="238" spans="1:2">
       <c r="A238" s="1">
@@ -2258,24 +2276,18 @@
       <c r="A239" s="1">
         <v>237</v>
       </c>
-      <c r="B239" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="240" spans="1:2">
       <c r="A240" s="1">
         <v>238</v>
       </c>
-      <c r="B240" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="241" spans="1:2">
       <c r="A241" s="1">
         <v>239</v>
       </c>
       <c r="B241" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="242" spans="1:2">
@@ -2298,7 +2310,7 @@
         <v>243</v>
       </c>
       <c r="B245" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="246" spans="1:2">
@@ -2321,7 +2333,7 @@
         <v>247</v>
       </c>
       <c r="B249" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="250" spans="1:2">
@@ -2344,7 +2356,7 @@
         <v>251</v>
       </c>
       <c r="B253" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="254" spans="1:2">
@@ -2367,18 +2379,24 @@
         <v>255</v>
       </c>
       <c r="B257" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="258" spans="1:2">
       <c r="A258" s="1">
         <v>256</v>
       </c>
+      <c r="B258" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="259" spans="1:2">
       <c r="A259" s="1">
         <v>257</v>
       </c>
+      <c r="B259" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="260" spans="1:2">
       <c r="A260" s="1">
@@ -2389,9 +2407,6 @@
       <c r="A261" s="1">
         <v>259</v>
       </c>
-      <c r="B261" t="s">
-        <v>104</v>
-      </c>
     </row>
     <row r="262" spans="1:2">
       <c r="A262" s="1">
@@ -2402,6 +2417,9 @@
       <c r="A263" s="1">
         <v>261</v>
       </c>
+      <c r="B263" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="264" spans="1:2">
       <c r="A264" s="1">
@@ -2412,9 +2430,6 @@
       <c r="A265" s="1">
         <v>263</v>
       </c>
-      <c r="B265" t="s">
-        <v>105</v>
-      </c>
     </row>
     <row r="266" spans="1:2">
       <c r="A266" s="1">
@@ -2425,6 +2440,9 @@
       <c r="A267" s="1">
         <v>265</v>
       </c>
+      <c r="B267" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="268" spans="1:2">
       <c r="A268" s="1">
@@ -2435,24 +2453,18 @@
       <c r="A269" s="1">
         <v>267</v>
       </c>
-      <c r="B269" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="270" spans="1:2">
       <c r="A270" s="1">
         <v>268</v>
       </c>
-      <c r="B270" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="271" spans="1:2">
       <c r="A271" s="1">
         <v>269</v>
       </c>
       <c r="B271" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="272" spans="1:2">
@@ -2475,24 +2487,18 @@
         <v>273</v>
       </c>
       <c r="B275" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="276" spans="1:2">
       <c r="A276" s="1">
         <v>274</v>
       </c>
-      <c r="B276" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="277" spans="1:2">
       <c r="A277" s="1">
         <v>275</v>
       </c>
-      <c r="B277" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="278" spans="1:2">
       <c r="A278" s="1">
@@ -2503,6 +2509,9 @@
       <c r="A279" s="1">
         <v>277</v>
       </c>
+      <c r="B279" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="280" spans="1:2">
       <c r="A280" s="1">
@@ -2513,24 +2522,18 @@
       <c r="A281" s="1">
         <v>279</v>
       </c>
-      <c r="B281" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="282" spans="1:2">
       <c r="A282" s="1">
         <v>280</v>
       </c>
-      <c r="B282" t="s">
-        <v>113</v>
-      </c>
     </row>
     <row r="283" spans="1:2">
       <c r="A283" s="1">
         <v>281</v>
       </c>
       <c r="B283" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="284" spans="1:2">
@@ -2553,7 +2556,7 @@
         <v>285</v>
       </c>
       <c r="B287" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="288" spans="1:2">
@@ -2576,7 +2579,7 @@
         <v>289</v>
       </c>
       <c r="B291" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="292" spans="1:2">
@@ -2599,18 +2602,24 @@
         <v>293</v>
       </c>
       <c r="B295" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="296" spans="1:2">
       <c r="A296" s="1">
         <v>294</v>
       </c>
+      <c r="B296" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="297" spans="1:2">
       <c r="A297" s="1">
         <v>295</v>
       </c>
+      <c r="B297" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="298" spans="1:2">
       <c r="A298" s="1">
@@ -2621,9 +2630,6 @@
       <c r="A299" s="1">
         <v>297</v>
       </c>
-      <c r="B299" t="s">
-        <v>118</v>
-      </c>
     </row>
     <row r="300" spans="1:2">
       <c r="A300" s="1">
@@ -2634,6 +2640,9 @@
       <c r="A301" s="1">
         <v>299</v>
       </c>
+      <c r="B301" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="302" spans="1:2">
       <c r="A302" s="1">
@@ -2644,9 +2653,6 @@
       <c r="A303" s="1">
         <v>301</v>
       </c>
-      <c r="B303" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="304" spans="1:2">
       <c r="A304" s="1">
@@ -2657,18 +2663,24 @@
       <c r="A305" s="1">
         <v>303</v>
       </c>
+      <c r="B305" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="306" spans="1:2">
       <c r="A306" s="1">
         <v>304</v>
       </c>
+      <c r="B306" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="307" spans="1:2">
       <c r="A307" s="1">
         <v>305</v>
       </c>
       <c r="B307" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="308" spans="1:2">
@@ -2691,18 +2703,24 @@
         <v>309</v>
       </c>
       <c r="B311" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="312" spans="1:2">
       <c r="A312" s="1">
         <v>310</v>
       </c>
+      <c r="B312" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="313" spans="1:2">
       <c r="A313" s="1">
         <v>311</v>
       </c>
+      <c r="B313" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="314" spans="1:2">
       <c r="A314" s="1">
@@ -2713,35 +2731,35 @@
       <c r="A315" s="1">
         <v>313</v>
       </c>
-      <c r="B315" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="316" spans="1:2">
       <c r="A316" s="1">
         <v>314</v>
       </c>
-      <c r="B316" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="317" spans="1:2">
       <c r="A317" s="1">
         <v>315</v>
       </c>
       <c r="B317" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="318" spans="1:2">
       <c r="A318" s="1">
         <v>316</v>
       </c>
+      <c r="B318" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="319" spans="1:2">
       <c r="A319" s="1">
         <v>317</v>
       </c>
+      <c r="B319" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="320" spans="1:2">
       <c r="A320" s="1">
@@ -2752,35 +2770,35 @@
       <c r="A321" s="1">
         <v>319</v>
       </c>
-      <c r="B321" t="s">
-        <v>125</v>
-      </c>
     </row>
     <row r="322" spans="1:2">
       <c r="A322" s="1">
         <v>320</v>
       </c>
-      <c r="B322" t="s">
-        <v>126</v>
-      </c>
     </row>
     <row r="323" spans="1:2">
       <c r="A323" s="1">
         <v>321</v>
       </c>
       <c r="B323" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="324" spans="1:2">
       <c r="A324" s="1">
         <v>322</v>
       </c>
+      <c r="B324" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="325" spans="1:2">
       <c r="A325" s="1">
         <v>323</v>
       </c>
+      <c r="B325" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="326" spans="1:2">
       <c r="A326" s="1">
@@ -2791,9 +2809,6 @@
       <c r="A327" s="1">
         <v>325</v>
       </c>
-      <c r="B327" t="s">
-        <v>128</v>
-      </c>
     </row>
     <row r="328" spans="1:2">
       <c r="A328" s="1">
@@ -2804,18 +2819,24 @@
       <c r="A329" s="1">
         <v>327</v>
       </c>
+      <c r="B329" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="330" spans="1:2">
       <c r="A330" s="1">
         <v>328</v>
       </c>
+      <c r="B330" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="331" spans="1:2">
       <c r="A331" s="1">
         <v>329</v>
       </c>
       <c r="B331" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="332" spans="1:2">
@@ -2831,29 +2852,6 @@
     <row r="334" spans="1:2">
       <c r="A334" s="1">
         <v>332</v>
-      </c>
-    </row>
-    <row r="335" spans="1:2">
-      <c r="A335" s="1">
-        <v>333</v>
-      </c>
-      <c r="B335" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="336" spans="1:2">
-      <c r="A336" s="1">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="337" spans="1:1">
-      <c r="A337" s="1">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="338" spans="1:1">
-      <c r="A338" s="1">
-        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>